<commit_message>
flinke opruimslag voor alle epi bestandjes en de nieuwe resultaten en visualizers toegevoegd
</commit_message>
<xml_diff>
--- a/epidemic model/6-sector/R0 for windowsize 100.xlsx
+++ b/epidemic model/6-sector/R0 for windowsize 100.xlsx
@@ -14,12 +14,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="7">
   <si>
     <t>NFB</t>
   </si>
   <si>
     <t>HH&amp;NP</t>
+  </si>
+  <si>
+    <t>DFS</t>
+  </si>
+  <si>
+    <t>W</t>
   </si>
   <si>
     <t>S&amp;LG</t>
@@ -28,10 +34,7 @@
     <t>FG</t>
   </si>
   <si>
-    <t>DFS</t>
-  </si>
-  <si>
-    <t>W</t>
+    <t>inf</t>
   </si>
 </sst>
 </file>
@@ -426,1471 +429,1471 @@
         <v>28125</v>
       </c>
       <c r="B2">
-        <v>2.26450756446188</v>
+        <v>2.1891918384449</v>
       </c>
       <c r="C2">
-        <v>3.09682179899305</v>
-      </c>
-      <c r="D2">
-        <v>6.6631816159165</v>
+        <v>2.23432846599536</v>
+      </c>
+      <c r="D2" t="s">
+        <v>6</v>
       </c>
       <c r="E2">
-        <v>3.04278827253712</v>
+        <v>4.62498660255844</v>
       </c>
       <c r="F2">
-        <v>3.20026968917809</v>
+        <v>4.3415893456895</v>
       </c>
       <c r="G2">
-        <v>4.97827045444304</v>
+        <v>1.72339190013131</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="2">
         <v>28215</v>
       </c>
-      <c r="B3">
-        <v>2.27886958214186</v>
+      <c r="B3" t="s">
+        <v>6</v>
       </c>
       <c r="C3">
-        <v>2.84175333389128</v>
-      </c>
-      <c r="D3">
-        <v>7.31647962217421</v>
+        <v>2.60693503800151</v>
+      </c>
+      <c r="D3" t="s">
+        <v>6</v>
       </c>
       <c r="E3">
-        <v>3.40113971473916</v>
+        <v>3.40342148022605</v>
       </c>
       <c r="F3">
-        <v>2.91366317896899</v>
+        <v>3.26291248143616</v>
       </c>
       <c r="G3">
-        <v>5.07743870128409</v>
+        <v>1.27087480539434</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" s="2">
         <v>28306</v>
       </c>
-      <c r="B4">
-        <v>1.83190720162391</v>
+      <c r="B4" t="s">
+        <v>6</v>
       </c>
       <c r="C4">
-        <v>2.85648083376606</v>
-      </c>
-      <c r="D4">
-        <v>6.36247539744904</v>
+        <v>2.21872032258911</v>
+      </c>
+      <c r="D4" t="s">
+        <v>6</v>
       </c>
       <c r="E4">
-        <v>3.0989799404292</v>
+        <v>3.76147934689369</v>
       </c>
       <c r="F4">
-        <v>2.8401867311048</v>
+        <v>3.62988857442524</v>
       </c>
       <c r="G4">
-        <v>4.63649868350649</v>
+        <v>1.34395564986591</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" s="2">
         <v>28398</v>
       </c>
-      <c r="B5">
-        <v>2.46383965551903</v>
+      <c r="B5" t="s">
+        <v>6</v>
       </c>
       <c r="C5">
-        <v>2.79471154287064</v>
-      </c>
-      <c r="D5">
-        <v>6.43468366209116</v>
+        <v>1.62756421942015</v>
+      </c>
+      <c r="D5" t="s">
+        <v>6</v>
       </c>
       <c r="E5">
-        <v>2.82442532990249</v>
+        <v>3.415079999189</v>
       </c>
       <c r="F5">
-        <v>2.87042726765569</v>
+        <v>3.32544707080805</v>
       </c>
       <c r="G5">
-        <v>4.92375100799415</v>
+        <v>1.17753647361733</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" s="2">
         <v>28490</v>
       </c>
-      <c r="B6">
-        <v>2.52332555206969</v>
+      <c r="B6" t="s">
+        <v>6</v>
       </c>
       <c r="C6">
-        <v>2.85608692782879</v>
-      </c>
-      <c r="D6">
-        <v>6.35739764836955</v>
+        <v>2.42515086153585</v>
+      </c>
+      <c r="D6" t="s">
+        <v>6</v>
       </c>
       <c r="E6">
-        <v>3.10723184373927</v>
+        <v>3.5226981287802</v>
       </c>
       <c r="F6">
-        <v>2.74319653863453</v>
+        <v>3.29336871396526</v>
       </c>
       <c r="G6">
-        <v>4.85498651948272</v>
+        <v>1.50728791677423</v>
       </c>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" s="2">
         <v>28580</v>
       </c>
-      <c r="B7">
-        <v>2.49839924717805</v>
+      <c r="B7" t="s">
+        <v>6</v>
       </c>
       <c r="C7">
-        <v>3.27133376366266</v>
-      </c>
-      <c r="D7">
-        <v>5.92989319359592</v>
+        <v>2.36422209978591</v>
+      </c>
+      <c r="D7" t="s">
+        <v>6</v>
       </c>
       <c r="E7">
-        <v>3.24681814444932</v>
+        <v>3.34215230494567</v>
       </c>
       <c r="F7">
-        <v>2.72774507771689</v>
+        <v>3.79255854142989</v>
       </c>
       <c r="G7">
-        <v>4.89367441954779</v>
+        <v>1.31808587923178</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="2">
         <v>28671</v>
       </c>
-      <c r="B8">
-        <v>2.58814869389123</v>
+      <c r="B8" t="s">
+        <v>6</v>
       </c>
       <c r="C8">
-        <v>3.05239074021681</v>
-      </c>
-      <c r="D8">
-        <v>6.09228021383384</v>
+        <v>1.86668001459564</v>
+      </c>
+      <c r="D8" t="s">
+        <v>6</v>
       </c>
       <c r="E8">
-        <v>2.93484810033657</v>
+        <v>4.1556749689377</v>
       </c>
       <c r="F8">
-        <v>2.81612743852913</v>
+        <v>3.73078387470773</v>
       </c>
       <c r="G8">
-        <v>4.48574003881267</v>
+        <v>1.32574632142131</v>
       </c>
     </row>
     <row r="9" spans="1:7">
       <c r="A9" s="2">
         <v>28763</v>
       </c>
-      <c r="B9">
-        <v>3.03792783598559</v>
+      <c r="B9" t="s">
+        <v>6</v>
       </c>
       <c r="C9">
-        <v>2.27102104179606</v>
-      </c>
-      <c r="D9">
-        <v>5.64195151079348</v>
+        <v>2.40674681276767</v>
+      </c>
+      <c r="D9" t="s">
+        <v>6</v>
       </c>
       <c r="E9">
-        <v>2.63354602062874</v>
+        <v>2.6326586594031</v>
       </c>
       <c r="F9">
-        <v>2.89596092269586</v>
+        <v>3.12314297172733</v>
       </c>
       <c r="G9">
-        <v>4.84559399247949</v>
+        <v>1.02311820490942</v>
       </c>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" s="2">
         <v>28855</v>
       </c>
-      <c r="B10">
-        <v>2.42701639720591</v>
+      <c r="B10" t="s">
+        <v>6</v>
       </c>
       <c r="C10">
-        <v>3.01657908395978</v>
-      </c>
-      <c r="D10">
-        <v>5.459488729662</v>
+        <v>1.56011048250342</v>
+      </c>
+      <c r="D10" t="s">
+        <v>6</v>
       </c>
       <c r="E10">
-        <v>3.13138079112712</v>
+        <v>3.80415136381335</v>
       </c>
       <c r="F10">
-        <v>2.8258647702167</v>
+        <v>2.50653706382721</v>
       </c>
       <c r="G10">
-        <v>4.93656651639029</v>
+        <v>1.72002905304363</v>
       </c>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="2">
         <v>28945</v>
       </c>
-      <c r="B11">
-        <v>2.37740861901072</v>
+      <c r="B11" t="s">
+        <v>6</v>
       </c>
       <c r="C11">
-        <v>3.00789041802497</v>
-      </c>
-      <c r="D11">
-        <v>5.4701165587976</v>
+        <v>2.31489413164927</v>
+      </c>
+      <c r="D11" t="s">
+        <v>6</v>
       </c>
       <c r="E11">
-        <v>3.06572846368924</v>
+        <v>3.00794061755505</v>
       </c>
       <c r="F11">
-        <v>2.84671868588733</v>
+        <v>2.73375143971315</v>
       </c>
       <c r="G11">
-        <v>5.18123102212323</v>
+        <v>1.37916850904074</v>
       </c>
     </row>
     <row r="12" spans="1:7">
       <c r="A12" s="2">
         <v>29036</v>
       </c>
-      <c r="B12">
-        <v>1.97683148701925</v>
+      <c r="B12" t="s">
+        <v>6</v>
       </c>
       <c r="C12">
-        <v>3.04844217379051</v>
-      </c>
-      <c r="D12">
-        <v>5.59371673683298</v>
+        <v>1.92311480325152</v>
+      </c>
+      <c r="D12" t="s">
+        <v>6</v>
       </c>
       <c r="E12">
-        <v>3.22499081261594</v>
+        <v>2.78489810980651</v>
       </c>
       <c r="F12">
-        <v>3.13546653955998</v>
+        <v>2.52206371404887</v>
       </c>
       <c r="G12">
-        <v>4.52477643780706</v>
+        <v>1.49518370339218</v>
       </c>
     </row>
     <row r="13" spans="1:7">
       <c r="A13" s="2">
         <v>29128</v>
       </c>
-      <c r="B13">
-        <v>2.22507287836646</v>
+      <c r="B13" t="s">
+        <v>6</v>
       </c>
       <c r="C13">
-        <v>3.20508646499531</v>
-      </c>
-      <c r="D13">
-        <v>5.90763419696332</v>
+        <v>2.03462476506791</v>
+      </c>
+      <c r="D13" t="s">
+        <v>6</v>
       </c>
       <c r="E13">
-        <v>3.32108966941903</v>
+        <v>3.1807995817572</v>
       </c>
       <c r="F13">
-        <v>3.18884969371411</v>
+        <v>2.61317746104467</v>
       </c>
       <c r="G13">
-        <v>4.656310707384</v>
+        <v>1.34789152032533</v>
       </c>
     </row>
     <row r="14" spans="1:7">
       <c r="A14" s="2">
         <v>29220</v>
       </c>
-      <c r="B14">
-        <v>2.23687336196179</v>
+      <c r="B14" t="s">
+        <v>6</v>
       </c>
       <c r="C14">
-        <v>3.11452229674645</v>
-      </c>
-      <c r="D14">
-        <v>6.27452062450762</v>
+        <v>2.10903885219278</v>
+      </c>
+      <c r="D14" t="s">
+        <v>6</v>
       </c>
       <c r="E14">
-        <v>3.32317135850753</v>
+        <v>3.09694911403394</v>
       </c>
       <c r="F14">
-        <v>2.49766442973633</v>
+        <v>2.77994765419076</v>
       </c>
       <c r="G14">
-        <v>4.91145870318043</v>
+        <v>1.36963340921717</v>
       </c>
     </row>
     <row r="15" spans="1:7">
       <c r="A15" s="2">
         <v>29311</v>
       </c>
-      <c r="B15">
-        <v>2.1952114195599</v>
+      <c r="B15" t="s">
+        <v>6</v>
       </c>
       <c r="C15">
-        <v>3.12701694370653</v>
-      </c>
-      <c r="D15">
-        <v>6.46239631894359</v>
+        <v>2.13466112453919</v>
+      </c>
+      <c r="D15" t="s">
+        <v>6</v>
       </c>
       <c r="E15">
-        <v>3.50818610209495</v>
+        <v>3.06379898911517</v>
       </c>
       <c r="F15">
-        <v>2.68563020526221</v>
+        <v>2.66772806987426</v>
       </c>
       <c r="G15">
-        <v>4.64711184622873</v>
+        <v>1.34977951248422</v>
       </c>
     </row>
     <row r="16" spans="1:7">
       <c r="A16" s="2">
         <v>29402</v>
       </c>
-      <c r="B16">
-        <v>2.20970564743606</v>
+      <c r="B16" t="s">
+        <v>6</v>
       </c>
       <c r="C16">
-        <v>3.07761761805121</v>
-      </c>
-      <c r="D16">
-        <v>6.79859361681492</v>
+        <v>2.24155883428354</v>
+      </c>
+      <c r="D16" t="s">
+        <v>6</v>
       </c>
       <c r="E16">
-        <v>3.29148488572486</v>
+        <v>3.0938198310035</v>
       </c>
       <c r="F16">
-        <v>2.81181392826273</v>
+        <v>2.31865722000685</v>
       </c>
       <c r="G16">
-        <v>4.69154078620316</v>
+        <v>1.27032144615686</v>
       </c>
     </row>
     <row r="17" spans="1:7">
       <c r="A17" s="2">
         <v>29494</v>
       </c>
-      <c r="B17">
-        <v>2.68958469200707</v>
+      <c r="B17" t="s">
+        <v>6</v>
       </c>
       <c r="C17">
-        <v>3.08661746441427</v>
-      </c>
-      <c r="D17">
-        <v>6.34762842899718</v>
+        <v>2.07286756136555</v>
+      </c>
+      <c r="D17" t="s">
+        <v>6</v>
       </c>
       <c r="E17">
-        <v>2.90920288937081</v>
+        <v>3.61732349613921</v>
       </c>
       <c r="F17">
-        <v>2.9662378315632</v>
+        <v>2.75097580584065</v>
       </c>
       <c r="G17">
-        <v>5.00508746044949</v>
+        <v>1.0297662696181</v>
       </c>
     </row>
     <row r="18" spans="1:7">
       <c r="A18" s="2">
         <v>29586</v>
       </c>
-      <c r="B18">
-        <v>3.35507414544686</v>
+      <c r="B18" t="s">
+        <v>6</v>
       </c>
       <c r="C18">
-        <v>3.08400436525706</v>
-      </c>
-      <c r="D18">
-        <v>5.9582374879772</v>
+        <v>2.01677423476064</v>
+      </c>
+      <c r="D18" t="s">
+        <v>6</v>
       </c>
       <c r="E18">
-        <v>2.59395472081659</v>
+        <v>3.4486830551639</v>
       </c>
       <c r="F18">
-        <v>2.65738126326412</v>
+        <v>2.25941324587523</v>
       </c>
       <c r="G18">
-        <v>4.70310926843237</v>
+        <v>1.24794045834352</v>
       </c>
     </row>
     <row r="19" spans="1:7">
       <c r="A19" s="2">
         <v>29676</v>
       </c>
-      <c r="B19">
-        <v>2.3872292672556</v>
+      <c r="B19" t="s">
+        <v>6</v>
       </c>
       <c r="C19">
-        <v>3.28101722331476</v>
-      </c>
-      <c r="D19">
-        <v>6.31215252412442</v>
+        <v>2.33599755459011</v>
+      </c>
+      <c r="D19" t="s">
+        <v>6</v>
       </c>
       <c r="E19">
-        <v>2.82833274270536</v>
+        <v>3.12737629519639</v>
       </c>
       <c r="F19">
-        <v>3.47557042880207</v>
+        <v>2.74031447745683</v>
       </c>
       <c r="G19">
-        <v>4.60339939072859</v>
+        <v>1.38282161502883</v>
       </c>
     </row>
     <row r="20" spans="1:7">
       <c r="A20" s="2">
         <v>29767</v>
       </c>
-      <c r="B20">
-        <v>2.52139251573078</v>
+      <c r="B20" t="s">
+        <v>6</v>
       </c>
       <c r="C20">
-        <v>2.93514183407105</v>
-      </c>
-      <c r="D20">
-        <v>7.06922573840748</v>
+        <v>2.27633956650783</v>
+      </c>
+      <c r="D20" t="s">
+        <v>6</v>
       </c>
       <c r="E20">
-        <v>2.92879038428293</v>
+        <v>3.20093063182943</v>
       </c>
       <c r="F20">
-        <v>3.35458528916911</v>
+        <v>2.69566293990871</v>
       </c>
       <c r="G20">
-        <v>4.35988157830239</v>
+        <v>1.28182531985532</v>
       </c>
     </row>
     <row r="21" spans="1:7">
       <c r="A21" s="2">
         <v>29859</v>
       </c>
-      <c r="B21">
-        <v>2.65311870036303</v>
+      <c r="B21" t="s">
+        <v>6</v>
       </c>
       <c r="C21">
-        <v>3.10855295980817</v>
-      </c>
-      <c r="D21">
-        <v>6.2504643494874</v>
+        <v>1.8373867010635</v>
+      </c>
+      <c r="D21" t="s">
+        <v>6</v>
       </c>
       <c r="E21">
-        <v>2.90901381872908</v>
+        <v>3.87420813622145</v>
       </c>
       <c r="F21">
-        <v>3.06820121422237</v>
+        <v>2.76189868547276</v>
       </c>
       <c r="G21">
-        <v>4.64743055009361</v>
+        <v>1.08732447210692</v>
       </c>
     </row>
     <row r="22" spans="1:7">
       <c r="A22" s="2">
         <v>29951</v>
       </c>
-      <c r="B22">
-        <v>2.4948347744794</v>
+      <c r="B22" t="s">
+        <v>6</v>
       </c>
       <c r="C22">
-        <v>3.38416393204495</v>
-      </c>
-      <c r="D22">
-        <v>6.49986214194817</v>
+        <v>2.0355248695306</v>
+      </c>
+      <c r="D22" t="s">
+        <v>6</v>
       </c>
       <c r="E22">
-        <v>2.873139673262</v>
+        <v>3.54822174860866</v>
       </c>
       <c r="F22">
-        <v>3.05182983536034</v>
+        <v>2.83499854729405</v>
       </c>
       <c r="G22">
-        <v>4.59681983528669</v>
+        <v>1.0993273405507</v>
       </c>
     </row>
     <row r="23" spans="1:7">
       <c r="A23" s="2">
         <v>30041</v>
       </c>
-      <c r="B23">
-        <v>2.47666599864187</v>
+      <c r="B23" t="s">
+        <v>6</v>
       </c>
       <c r="C23">
-        <v>2.9819695939239</v>
-      </c>
-      <c r="D23">
-        <v>6.18482824049937</v>
+        <v>2.01249287745339</v>
+      </c>
+      <c r="D23" t="s">
+        <v>6</v>
       </c>
       <c r="E23">
-        <v>2.78762838591387</v>
+        <v>3.38007113707112</v>
       </c>
       <c r="F23">
-        <v>3.2887568270303</v>
+        <v>2.52591781225968</v>
       </c>
       <c r="G23">
-        <v>4.6497344732055</v>
+        <v>1.22803318355205</v>
       </c>
     </row>
     <row r="24" spans="1:7">
       <c r="A24" s="2">
         <v>30132</v>
       </c>
-      <c r="B24">
-        <v>2.56113404707684</v>
+      <c r="B24" t="s">
+        <v>6</v>
       </c>
       <c r="C24">
-        <v>2.94812049864668</v>
-      </c>
-      <c r="D24">
-        <v>6.52089620745972</v>
+        <v>2.28788890503303</v>
+      </c>
+      <c r="D24" t="s">
+        <v>6</v>
       </c>
       <c r="E24">
-        <v>2.84029389595017</v>
+        <v>2.72852134709931</v>
       </c>
       <c r="F24">
-        <v>3.55885553760768</v>
+        <v>2.39427465179599</v>
       </c>
       <c r="G24">
-        <v>4.93784730554872</v>
+        <v>0.983205509774067</v>
       </c>
     </row>
     <row r="25" spans="1:7">
       <c r="A25" s="2">
         <v>30224</v>
       </c>
-      <c r="B25">
-        <v>2.840211006288</v>
+      <c r="B25" t="s">
+        <v>6</v>
       </c>
       <c r="C25">
-        <v>3.04161706092333</v>
-      </c>
-      <c r="D25">
-        <v>6.66656681773932</v>
+        <v>1.86110042741422</v>
+      </c>
+      <c r="D25" t="s">
+        <v>6</v>
       </c>
       <c r="E25">
-        <v>2.73781620961722</v>
+        <v>3.44150915491645</v>
       </c>
       <c r="F25">
-        <v>3.36275899423818</v>
+        <v>2.90954019919962</v>
       </c>
       <c r="G25">
-        <v>4.13198949553805</v>
+        <v>1.25847280403991</v>
       </c>
     </row>
     <row r="26" spans="1:7">
       <c r="A26" s="2">
         <v>30316</v>
       </c>
-      <c r="B26">
-        <v>2.84224597998541</v>
+      <c r="B26" t="s">
+        <v>6</v>
       </c>
       <c r="C26">
-        <v>3.17584050396783</v>
-      </c>
-      <c r="D26">
-        <v>6.53381311227221</v>
+        <v>2.13499912646477</v>
+      </c>
+      <c r="D26" t="s">
+        <v>6</v>
       </c>
       <c r="E26">
-        <v>2.86534709794725</v>
+        <v>4.37202379392679</v>
       </c>
       <c r="F26">
-        <v>3.4649757656378</v>
+        <v>1.9022125820784</v>
       </c>
       <c r="G26">
-        <v>3.73079665217762</v>
+        <v>1.46417617184622</v>
       </c>
     </row>
     <row r="27" spans="1:7">
       <c r="A27" s="2">
         <v>30406</v>
       </c>
-      <c r="B27">
-        <v>2.80528160976411</v>
+      <c r="B27" t="s">
+        <v>6</v>
       </c>
       <c r="C27">
-        <v>3.24166665266767</v>
-      </c>
-      <c r="D27">
-        <v>6.49143139179991</v>
+        <v>2.01398344899478</v>
+      </c>
+      <c r="D27" t="s">
+        <v>6</v>
       </c>
       <c r="E27">
-        <v>2.83965811246381</v>
+        <v>3.59333537326407</v>
       </c>
       <c r="F27">
-        <v>3.66490400543933</v>
+        <v>2.08098174186171</v>
       </c>
       <c r="G27">
-        <v>3.53383292560927</v>
+        <v>1.54132072654427</v>
       </c>
     </row>
     <row r="28" spans="1:7">
       <c r="A28" s="2">
         <v>30497</v>
       </c>
-      <c r="B28">
-        <v>2.82189401570086</v>
+      <c r="B28" t="s">
+        <v>6</v>
       </c>
       <c r="C28">
-        <v>2.89954509622205</v>
-      </c>
-      <c r="D28">
-        <v>6.68542170087625</v>
+        <v>2.05446302191817</v>
+      </c>
+      <c r="D28" t="s">
+        <v>6</v>
       </c>
       <c r="E28">
-        <v>3.04815561744862</v>
+        <v>3.98770397514909</v>
       </c>
       <c r="F28">
-        <v>3.55020237447917</v>
+        <v>2.17934140155846</v>
       </c>
       <c r="G28">
-        <v>3.31071308970826</v>
+        <v>1.28905332144327</v>
       </c>
     </row>
     <row r="29" spans="1:7">
       <c r="A29" s="2">
         <v>30589</v>
       </c>
-      <c r="B29">
-        <v>3.15701179986756</v>
+      <c r="B29" t="s">
+        <v>6</v>
       </c>
       <c r="C29">
-        <v>2.66721341354496</v>
-      </c>
-      <c r="D29">
-        <v>6.34362761952289</v>
+        <v>2.12700946795191</v>
+      </c>
+      <c r="D29" t="s">
+        <v>6</v>
       </c>
       <c r="E29">
-        <v>2.90820334895209</v>
+        <v>3.63225199855955</v>
       </c>
       <c r="F29">
-        <v>3.51343901252666</v>
+        <v>2.1362885454628</v>
       </c>
       <c r="G29">
-        <v>3.37805109246795</v>
+        <v>1.52270992521657</v>
       </c>
     </row>
     <row r="30" spans="1:7">
       <c r="A30" s="2">
         <v>30681</v>
       </c>
-      <c r="B30">
-        <v>3.13697363429454</v>
+      <c r="B30" t="s">
+        <v>6</v>
       </c>
       <c r="C30">
-        <v>2.6919923501911</v>
-      </c>
-      <c r="D30">
-        <v>6.14320392608383</v>
+        <v>2.24410891736098</v>
+      </c>
+      <c r="D30" t="s">
+        <v>6</v>
       </c>
       <c r="E30">
-        <v>2.80480029467158</v>
+        <v>3.43607250661443</v>
       </c>
       <c r="F30">
-        <v>3.39887393017595</v>
+        <v>2.2008097676279</v>
       </c>
       <c r="G30">
-        <v>3.29465996660644</v>
+        <v>1.48075996408414</v>
       </c>
     </row>
     <row r="31" spans="1:7">
       <c r="A31" s="2">
         <v>30772</v>
       </c>
-      <c r="B31">
-        <v>3.12637378743391</v>
+      <c r="B31" t="s">
+        <v>6</v>
       </c>
       <c r="C31">
-        <v>2.61658161053783</v>
-      </c>
-      <c r="D31">
-        <v>6.16987131672651</v>
+        <v>1.97551097115907</v>
+      </c>
+      <c r="D31" t="s">
+        <v>6</v>
       </c>
       <c r="E31">
-        <v>3.20508724913166</v>
+        <v>2.96447823122006</v>
       </c>
       <c r="F31">
-        <v>3.40983248730549</v>
+        <v>2.21092380703401</v>
       </c>
       <c r="G31">
-        <v>3.71415819236107</v>
+        <v>1.54340695656247</v>
       </c>
     </row>
     <row r="32" spans="1:7">
       <c r="A32" s="2">
         <v>30863</v>
       </c>
-      <c r="B32">
-        <v>3.06161441159022</v>
+      <c r="B32" t="s">
+        <v>6</v>
       </c>
       <c r="C32">
-        <v>2.60223718794361</v>
-      </c>
-      <c r="D32">
-        <v>6.29726928236395</v>
+        <v>2.19710185988626</v>
+      </c>
+      <c r="D32" t="s">
+        <v>6</v>
       </c>
       <c r="E32">
-        <v>3.22881777222246</v>
+        <v>2.97411257667131</v>
       </c>
       <c r="F32">
-        <v>3.45996266323239</v>
+        <v>2.07642302239401</v>
       </c>
       <c r="G32">
-        <v>3.16051135004239</v>
+        <v>1.51334326333291</v>
       </c>
     </row>
     <row r="33" spans="1:7">
       <c r="A33" s="2">
         <v>30955</v>
       </c>
-      <c r="B33">
-        <v>2.97249556772684</v>
+      <c r="B33" t="s">
+        <v>6</v>
       </c>
       <c r="C33">
-        <v>2.6193199685866</v>
-      </c>
-      <c r="D33">
-        <v>6.18814428746447</v>
+        <v>1.91394808099859</v>
+      </c>
+      <c r="D33" t="s">
+        <v>6</v>
       </c>
       <c r="E33">
-        <v>3.26127380140378</v>
-      </c>
-      <c r="F33">
-        <v>3.40753457873348</v>
+        <v>2.53024252404126</v>
+      </c>
+      <c r="F33" t="s">
+        <v>6</v>
       </c>
       <c r="G33">
-        <v>3.14988598376359</v>
+        <v>0.802975367831375</v>
       </c>
     </row>
     <row r="34" spans="1:7">
       <c r="A34" s="2">
         <v>31047</v>
       </c>
-      <c r="B34">
-        <v>3.00657242842154</v>
+      <c r="B34" t="s">
+        <v>6</v>
       </c>
       <c r="C34">
-        <v>2.63880654077413</v>
-      </c>
-      <c r="D34">
-        <v>6.26185610383021</v>
+        <v>2.20546587943184</v>
+      </c>
+      <c r="D34" t="s">
+        <v>6</v>
       </c>
       <c r="E34">
-        <v>3.2658690230125</v>
-      </c>
-      <c r="F34">
-        <v>3.41177278131047</v>
+        <v>2.52490494824702</v>
+      </c>
+      <c r="F34" t="s">
+        <v>6</v>
       </c>
       <c r="G34">
-        <v>3.09584693901633</v>
+        <v>1.07903746949842</v>
       </c>
     </row>
     <row r="35" spans="1:7">
       <c r="A35" s="2">
         <v>31137</v>
       </c>
-      <c r="B35">
-        <v>3.11592608117502</v>
+      <c r="B35" t="s">
+        <v>6</v>
       </c>
       <c r="C35">
-        <v>2.70147404611003</v>
-      </c>
-      <c r="D35">
-        <v>6.1295940486897</v>
+        <v>2.04293305331365</v>
+      </c>
+      <c r="D35" t="s">
+        <v>6</v>
       </c>
       <c r="E35">
-        <v>3.39319582626789</v>
-      </c>
-      <c r="F35">
-        <v>3.47503687163877</v>
+        <v>2.34500006349571</v>
+      </c>
+      <c r="F35" t="s">
+        <v>6</v>
       </c>
       <c r="G35">
-        <v>3.10092217602985</v>
+        <v>1.02430996180122</v>
       </c>
     </row>
     <row r="36" spans="1:7">
       <c r="A36" s="2">
         <v>31228</v>
       </c>
-      <c r="B36">
-        <v>3.13130098429562</v>
+      <c r="B36" t="s">
+        <v>6</v>
       </c>
       <c r="C36">
-        <v>2.74317204814728</v>
-      </c>
-      <c r="D36">
-        <v>5.94041724337261</v>
+        <v>1.87701660005447</v>
+      </c>
+      <c r="D36" t="s">
+        <v>6</v>
       </c>
       <c r="E36">
-        <v>3.37019548129175</v>
-      </c>
-      <c r="F36">
-        <v>3.33851030855455</v>
+        <v>2.50578852457858</v>
+      </c>
+      <c r="F36" t="s">
+        <v>6</v>
       </c>
       <c r="G36">
-        <v>3.17598171886871</v>
+        <v>0.737834723405425</v>
       </c>
     </row>
     <row r="37" spans="1:7">
       <c r="A37" s="2">
         <v>31320</v>
       </c>
-      <c r="B37">
-        <v>3.07931558054236</v>
+      <c r="B37" t="s">
+        <v>6</v>
       </c>
       <c r="C37">
-        <v>2.60146663050542</v>
-      </c>
-      <c r="D37">
-        <v>6.07335396238296</v>
+        <v>1.97306151567317</v>
+      </c>
+      <c r="D37" t="s">
+        <v>6</v>
       </c>
       <c r="E37">
-        <v>3.49985695936033</v>
-      </c>
-      <c r="F37">
-        <v>3.38122553176956</v>
+        <v>2.37311511233359</v>
+      </c>
+      <c r="F37" t="s">
+        <v>6</v>
       </c>
       <c r="G37">
-        <v>3.38883555902302</v>
+        <v>1.04890887118582</v>
       </c>
     </row>
     <row r="38" spans="1:7">
       <c r="A38" s="2">
         <v>31412</v>
       </c>
-      <c r="B38">
-        <v>2.92070265963024</v>
+      <c r="B38" t="s">
+        <v>6</v>
       </c>
       <c r="C38">
-        <v>2.58877909034223</v>
-      </c>
-      <c r="D38">
-        <v>5.91092943842551</v>
+        <v>1.98261766035651</v>
+      </c>
+      <c r="D38" t="s">
+        <v>6</v>
       </c>
       <c r="E38">
-        <v>3.52509024491882</v>
-      </c>
-      <c r="F38">
-        <v>3.30348992291366</v>
+        <v>2.64985821173841</v>
+      </c>
+      <c r="F38" t="s">
+        <v>6</v>
       </c>
       <c r="G38">
-        <v>3.26761702777825</v>
+        <v>1.00757311778486</v>
       </c>
     </row>
     <row r="39" spans="1:7">
       <c r="A39" s="2">
         <v>31502</v>
       </c>
-      <c r="B39">
-        <v>3.04265768181411</v>
+      <c r="B39" t="s">
+        <v>6</v>
       </c>
       <c r="C39">
-        <v>2.69043543647217</v>
-      </c>
-      <c r="D39">
-        <v>5.93512506868128</v>
+        <v>2.32783443229917</v>
+      </c>
+      <c r="D39" t="s">
+        <v>6</v>
       </c>
       <c r="E39">
-        <v>3.44540261390041</v>
-      </c>
-      <c r="F39">
-        <v>3.21379380566524</v>
+        <v>1.87046149029557</v>
+      </c>
+      <c r="F39" t="s">
+        <v>6</v>
       </c>
       <c r="G39">
-        <v>3.33743249874101</v>
+        <v>0.892378002322392</v>
       </c>
     </row>
     <row r="40" spans="1:7">
       <c r="A40" s="2">
         <v>31593</v>
       </c>
-      <c r="B40">
-        <v>3.02008686428958</v>
+      <c r="B40" t="s">
+        <v>6</v>
       </c>
       <c r="C40">
-        <v>2.66817783730355</v>
-      </c>
-      <c r="D40">
-        <v>5.91003891350463</v>
+        <v>2.09198249167846</v>
+      </c>
+      <c r="D40" t="s">
+        <v>6</v>
       </c>
       <c r="E40">
-        <v>3.40555967575385</v>
-      </c>
-      <c r="F40">
-        <v>3.42654108940843</v>
+        <v>2.13213334336285</v>
+      </c>
+      <c r="F40" t="s">
+        <v>6</v>
       </c>
       <c r="G40">
-        <v>3.41350433730994</v>
+        <v>1.06393095385047</v>
       </c>
     </row>
     <row r="41" spans="1:7">
       <c r="A41" s="2">
         <v>31685</v>
       </c>
-      <c r="B41">
-        <v>3.29750263536814</v>
+      <c r="B41" t="s">
+        <v>6</v>
       </c>
       <c r="C41">
-        <v>2.49984492341001</v>
-      </c>
-      <c r="D41">
-        <v>5.229852875365</v>
+        <v>1.72239251750812</v>
+      </c>
+      <c r="D41" t="s">
+        <v>6</v>
       </c>
       <c r="E41">
-        <v>3.27781736435447</v>
-      </c>
-      <c r="F41">
-        <v>3.38174863533513</v>
+        <v>2.75191779128214</v>
+      </c>
+      <c r="F41" t="s">
+        <v>6</v>
       </c>
       <c r="G41">
-        <v>3.29548181653447</v>
+        <v>0.826143502513871</v>
       </c>
     </row>
     <row r="42" spans="1:7">
       <c r="A42" s="2">
         <v>31777</v>
       </c>
-      <c r="B42">
-        <v>2.96615348741449</v>
+      <c r="B42" t="s">
+        <v>6</v>
       </c>
       <c r="C42">
-        <v>2.27435582092314</v>
-      </c>
-      <c r="D42">
-        <v>5.46374549185427</v>
+        <v>2.12036078799905</v>
+      </c>
+      <c r="D42" t="s">
+        <v>6</v>
       </c>
       <c r="E42">
-        <v>3.2758979547617</v>
-      </c>
-      <c r="F42">
-        <v>3.46651169111466</v>
+        <v>2.44213238289424</v>
+      </c>
+      <c r="F42" t="s">
+        <v>6</v>
       </c>
       <c r="G42">
-        <v>3.66954935115722</v>
+        <v>1.08984328966123</v>
       </c>
     </row>
     <row r="43" spans="1:7">
       <c r="A43" s="2">
         <v>31867</v>
       </c>
-      <c r="B43">
-        <v>2.81859465380073</v>
+      <c r="B43" t="s">
+        <v>6</v>
       </c>
       <c r="C43">
-        <v>2.96398585159357</v>
-      </c>
-      <c r="D43">
-        <v>5.50138681190075</v>
+        <v>1.99809263881724</v>
+      </c>
+      <c r="D43" t="s">
+        <v>6</v>
       </c>
       <c r="E43">
-        <v>3.69923790589973</v>
-      </c>
-      <c r="F43">
-        <v>3.15773418804096</v>
+        <v>2.15864442609336</v>
+      </c>
+      <c r="F43" t="s">
+        <v>6</v>
       </c>
       <c r="G43">
-        <v>3.69315496138688</v>
+        <v>1.08036758640374</v>
       </c>
     </row>
     <row r="44" spans="1:7">
       <c r="A44" s="2">
         <v>31958</v>
       </c>
-      <c r="B44">
-        <v>2.83621156726611</v>
+      <c r="B44" t="s">
+        <v>6</v>
       </c>
       <c r="C44">
-        <v>1.13730001493873</v>
-      </c>
-      <c r="D44">
-        <v>6.66653009212008</v>
+        <v>2.08767216057785</v>
+      </c>
+      <c r="D44" t="s">
+        <v>6</v>
       </c>
       <c r="E44">
-        <v>3.22381312531705</v>
-      </c>
-      <c r="F44">
-        <v>1.93323544724165</v>
+        <v>2.45955291000469</v>
+      </c>
+      <c r="F44" t="s">
+        <v>6</v>
       </c>
       <c r="G44">
-        <v>3.33944575515369</v>
+        <v>1.08140822250565</v>
       </c>
     </row>
     <row r="45" spans="1:7">
       <c r="A45" s="2">
         <v>32050</v>
       </c>
-      <c r="B45">
-        <v>3.23665659566422</v>
+      <c r="B45" t="s">
+        <v>6</v>
       </c>
       <c r="C45">
-        <v>2.74481627998561</v>
-      </c>
-      <c r="D45">
-        <v>4.97732590593577</v>
+        <v>1.98286497469482</v>
+      </c>
+      <c r="D45" t="s">
+        <v>6</v>
       </c>
       <c r="E45">
-        <v>3.19787393570651</v>
-      </c>
-      <c r="F45">
-        <v>3.10534049595407</v>
+        <v>2.29544361444365</v>
+      </c>
+      <c r="F45" t="s">
+        <v>6</v>
       </c>
       <c r="G45">
-        <v>4.43564029573284</v>
+        <v>1.07858248880968</v>
       </c>
     </row>
     <row r="46" spans="1:7">
       <c r="A46" s="2">
         <v>32142</v>
       </c>
-      <c r="B46">
-        <v>3.23602075033286</v>
+      <c r="B46" t="s">
+        <v>6</v>
       </c>
       <c r="C46">
-        <v>1.86719798500106</v>
-      </c>
-      <c r="D46">
-        <v>5.22953814448377</v>
+        <v>1.68735565556844</v>
+      </c>
+      <c r="D46" t="s">
+        <v>6</v>
       </c>
       <c r="E46">
-        <v>3.70135148410234</v>
-      </c>
-      <c r="F46">
-        <v>2.14078943206928</v>
+        <v>2.20595061652899</v>
+      </c>
+      <c r="F46" t="s">
+        <v>6</v>
       </c>
       <c r="G46">
-        <v>4.7917739330613</v>
+        <v>1.23224892271495</v>
       </c>
     </row>
     <row r="47" spans="1:7">
       <c r="A47" s="2">
         <v>32233</v>
       </c>
-      <c r="B47">
-        <v>2.95820340339828</v>
+      <c r="B47" t="s">
+        <v>6</v>
       </c>
       <c r="C47">
-        <v>2.48229038484233</v>
-      </c>
-      <c r="D47">
-        <v>5.00322441577495</v>
+        <v>1.91294249684448</v>
+      </c>
+      <c r="D47" t="s">
+        <v>6</v>
       </c>
       <c r="E47">
-        <v>3.38162571001208</v>
-      </c>
-      <c r="F47">
-        <v>2.82131282162191</v>
+        <v>2.09958264357964</v>
+      </c>
+      <c r="F47" t="s">
+        <v>6</v>
       </c>
       <c r="G47">
-        <v>3.98303799893182</v>
+        <v>1.16615886751438</v>
       </c>
     </row>
     <row r="48" spans="1:7">
       <c r="A48" s="2">
         <v>32324</v>
       </c>
-      <c r="B48">
-        <v>2.95707429442433</v>
+      <c r="B48" t="s">
+        <v>6</v>
       </c>
       <c r="C48">
-        <v>2.96765574504111</v>
-      </c>
-      <c r="D48">
-        <v>4.86146829050115</v>
+        <v>2.21647046513301</v>
+      </c>
+      <c r="D48" t="s">
+        <v>6</v>
       </c>
       <c r="E48">
-        <v>3.55456712954869</v>
-      </c>
-      <c r="F48">
-        <v>3.11132120448224</v>
+        <v>2.28237759965335</v>
+      </c>
+      <c r="F48" t="s">
+        <v>6</v>
       </c>
       <c r="G48">
-        <v>3.92589396607271</v>
+        <v>1.22958160794835</v>
       </c>
     </row>
     <row r="49" spans="1:7">
       <c r="A49" s="2">
         <v>32416</v>
       </c>
-      <c r="B49">
-        <v>3.04040822880706</v>
+      <c r="B49" t="s">
+        <v>6</v>
       </c>
       <c r="C49">
-        <v>3.34423697520067</v>
-      </c>
-      <c r="D49">
-        <v>4.95923759973165</v>
+        <v>1.92031808588637</v>
+      </c>
+      <c r="D49" t="s">
+        <v>6</v>
       </c>
       <c r="E49">
-        <v>3.3724337764418</v>
-      </c>
-      <c r="F49">
-        <v>3.59378629860379</v>
+        <v>1.81517423510693</v>
+      </c>
+      <c r="F49" t="s">
+        <v>6</v>
       </c>
       <c r="G49">
-        <v>3.8488314385219</v>
+        <v>1.08878062976626</v>
       </c>
     </row>
     <row r="50" spans="1:7">
       <c r="A50" s="2">
         <v>32508</v>
       </c>
-      <c r="B50">
-        <v>4.25896468801692</v>
+      <c r="B50" t="s">
+        <v>6</v>
       </c>
       <c r="C50">
-        <v>1.24897664816565</v>
-      </c>
-      <c r="D50">
-        <v>4.58688318764726</v>
+        <v>2.03531015644269</v>
+      </c>
+      <c r="D50" t="s">
+        <v>6</v>
       </c>
       <c r="E50">
-        <v>3.35846506117523</v>
-      </c>
-      <c r="F50">
-        <v>2.87211296751608</v>
+        <v>2.13918227494294</v>
+      </c>
+      <c r="F50" t="s">
+        <v>6</v>
       </c>
       <c r="G50">
-        <v>3.18278812188786</v>
+        <v>1.13351843310817</v>
       </c>
     </row>
     <row r="51" spans="1:7">
       <c r="A51" s="2">
         <v>32598</v>
       </c>
-      <c r="B51">
-        <v>3.09212709441605</v>
+      <c r="B51" t="s">
+        <v>6</v>
       </c>
       <c r="C51">
-        <v>3.03708346538943</v>
-      </c>
-      <c r="D51">
-        <v>5.11061459661151</v>
+        <v>2.0608590637318</v>
+      </c>
+      <c r="D51" t="s">
+        <v>6</v>
       </c>
       <c r="E51">
-        <v>3.27513454055668</v>
-      </c>
-      <c r="F51">
-        <v>2.70593483216123</v>
+        <v>2.08059800407172</v>
+      </c>
+      <c r="F51" t="s">
+        <v>6</v>
       </c>
       <c r="G51">
-        <v>3.53943109556435</v>
+        <v>1.28382706571426</v>
       </c>
     </row>
     <row r="52" spans="1:7">
       <c r="A52" s="2">
         <v>32689</v>
       </c>
-      <c r="B52">
-        <v>2.92764725136566</v>
+      <c r="B52" t="s">
+        <v>6</v>
       </c>
       <c r="C52">
-        <v>3.12193392097254</v>
-      </c>
-      <c r="D52">
-        <v>5.29640868735249</v>
+        <v>1.85111899430815</v>
+      </c>
+      <c r="D52" t="s">
+        <v>6</v>
       </c>
       <c r="E52">
-        <v>3.21705924998165</v>
-      </c>
-      <c r="F52">
-        <v>3.12190978774385</v>
+        <v>2.48456855076216</v>
+      </c>
+      <c r="F52" t="s">
+        <v>6</v>
       </c>
       <c r="G52">
-        <v>4.14124541241712</v>
+        <v>1.14906381464682</v>
       </c>
     </row>
     <row r="53" spans="1:7">
       <c r="A53" s="2">
         <v>32781</v>
       </c>
-      <c r="B53">
-        <v>2.75301298514778</v>
+      <c r="B53" t="s">
+        <v>6</v>
       </c>
       <c r="C53">
-        <v>3.24956897759191</v>
-      </c>
-      <c r="D53">
-        <v>5.37101742494423</v>
+        <v>1.98181345331387</v>
+      </c>
+      <c r="D53" t="s">
+        <v>6</v>
       </c>
       <c r="E53">
-        <v>3.00779821202132</v>
-      </c>
-      <c r="F53">
-        <v>3.22395463311429</v>
+        <v>2.20219512293039</v>
+      </c>
+      <c r="F53" t="s">
+        <v>6</v>
       </c>
       <c r="G53">
-        <v>3.47166052371616</v>
+        <v>1.29242462274682</v>
       </c>
     </row>
     <row r="54" spans="1:7">
       <c r="A54" s="2">
         <v>32873</v>
       </c>
-      <c r="B54">
-        <v>2.95505811530991</v>
+      <c r="B54" t="s">
+        <v>6</v>
       </c>
       <c r="C54">
-        <v>2.99961632686935</v>
-      </c>
-      <c r="D54">
-        <v>4.95742818069557</v>
+        <v>1.98255810223083</v>
+      </c>
+      <c r="D54" t="s">
+        <v>6</v>
       </c>
       <c r="E54">
-        <v>3.8429299536639</v>
-      </c>
-      <c r="F54">
-        <v>2.86042960045468</v>
+        <v>2.24229774225039</v>
+      </c>
+      <c r="F54" t="s">
+        <v>6</v>
       </c>
       <c r="G54">
-        <v>4.37335418350394</v>
+        <v>1.33298105855602</v>
       </c>
     </row>
     <row r="55" spans="1:7">
       <c r="A55" s="2">
         <v>32963</v>
       </c>
-      <c r="B55">
-        <v>2.47983920790007</v>
+      <c r="B55" t="s">
+        <v>6</v>
       </c>
       <c r="C55">
-        <v>3.11484384162296</v>
-      </c>
-      <c r="D55">
-        <v>3.97892044953636</v>
+        <v>2.29078045981101</v>
+      </c>
+      <c r="D55" t="s">
+        <v>6</v>
       </c>
       <c r="E55">
-        <v>2.77619162413477</v>
-      </c>
-      <c r="F55">
-        <v>2.26138610112973</v>
+        <v>2.20608493004896</v>
+      </c>
+      <c r="F55" t="s">
+        <v>6</v>
       </c>
       <c r="G55">
-        <v>4.56939663033187</v>
+        <v>0.916371211022552</v>
       </c>
     </row>
     <row r="56" spans="1:7">
       <c r="A56" s="2">
         <v>33054</v>
       </c>
-      <c r="B56">
-        <v>2.87966296244808</v>
+      <c r="B56" t="s">
+        <v>6</v>
       </c>
       <c r="C56">
-        <v>2.00820410654471</v>
-      </c>
-      <c r="D56">
-        <v>5.97693372383873</v>
+        <v>2.02878719206201</v>
+      </c>
+      <c r="D56" t="s">
+        <v>6</v>
       </c>
       <c r="E56">
-        <v>3.82125674509824</v>
-      </c>
-      <c r="F56">
-        <v>2.65953637712795</v>
+        <v>2.31296293856378</v>
+      </c>
+      <c r="F56" t="s">
+        <v>6</v>
       </c>
       <c r="G56">
-        <v>4.20326217214557</v>
+        <v>1.29621867577603</v>
       </c>
     </row>
     <row r="57" spans="1:7">
       <c r="A57" s="2">
         <v>33146</v>
       </c>
-      <c r="B57">
-        <v>2.64669609164925</v>
+      <c r="B57" t="s">
+        <v>6</v>
       </c>
       <c r="C57">
-        <v>2.97171650551238</v>
-      </c>
-      <c r="D57">
-        <v>6.51019427087499</v>
+        <v>2.01320396728027</v>
+      </c>
+      <c r="D57" t="s">
+        <v>6</v>
       </c>
       <c r="E57">
-        <v>3.78143061468752</v>
-      </c>
-      <c r="F57">
-        <v>3.01155704666842</v>
+        <v>2.29039474442878</v>
+      </c>
+      <c r="F57" t="s">
+        <v>6</v>
       </c>
       <c r="G57">
-        <v>4.36051597145127</v>
+        <v>1.28646511563637</v>
       </c>
     </row>
     <row r="58" spans="1:7">
       <c r="A58" s="2">
         <v>33238</v>
       </c>
-      <c r="B58">
-        <v>3.15353981388726</v>
+      <c r="B58" t="s">
+        <v>6</v>
       </c>
       <c r="C58">
-        <v>3.06068784234823</v>
-      </c>
-      <c r="D58">
-        <v>6.09314297806483</v>
+        <v>1.94576365808089</v>
+      </c>
+      <c r="D58" t="s">
+        <v>6</v>
       </c>
       <c r="E58">
-        <v>3.35963163781842</v>
-      </c>
-      <c r="F58">
-        <v>2.85618974984142</v>
+        <v>2.07350666211544</v>
+      </c>
+      <c r="F58" t="s">
+        <v>6</v>
       </c>
       <c r="G58">
-        <v>4.40962726447396</v>
+        <v>1.39755987494812</v>
       </c>
     </row>
     <row r="59" spans="1:7">
       <c r="A59" s="2">
         <v>33328</v>
       </c>
-      <c r="B59">
-        <v>3.62210819618125</v>
+      <c r="B59" t="s">
+        <v>6</v>
       </c>
       <c r="C59">
-        <v>2.52161843267749</v>
-      </c>
-      <c r="D59">
-        <v>5.74464606132256</v>
+        <v>2.13057446036967</v>
+      </c>
+      <c r="D59" t="s">
+        <v>6</v>
       </c>
       <c r="E59">
-        <v>3.06147803910557</v>
-      </c>
-      <c r="F59">
-        <v>3.37896686865049</v>
+        <v>1.98731470697563</v>
+      </c>
+      <c r="F59" t="s">
+        <v>6</v>
       </c>
       <c r="G59">
-        <v>4.09970122368906</v>
+        <v>1.46246729257148</v>
       </c>
     </row>
     <row r="60" spans="1:7">
       <c r="A60" s="2">
         <v>33419</v>
       </c>
-      <c r="B60">
-        <v>2.54694136477656</v>
+      <c r="B60" t="s">
+        <v>6</v>
       </c>
       <c r="C60">
-        <v>2.42046638492449</v>
-      </c>
-      <c r="D60">
-        <v>6.1832296127829</v>
+        <v>1.78902493003369</v>
+      </c>
+      <c r="D60" t="s">
+        <v>6</v>
       </c>
       <c r="E60">
-        <v>3.58309547740782</v>
-      </c>
-      <c r="F60">
-        <v>3.30611525271872</v>
+        <v>1.91131961210478</v>
+      </c>
+      <c r="F60" t="s">
+        <v>6</v>
       </c>
       <c r="G60">
-        <v>3.63604847998982</v>
+        <v>1.33589168863988</v>
       </c>
     </row>
     <row r="61" spans="1:7">
       <c r="A61" s="2">
         <v>33511</v>
       </c>
-      <c r="B61">
-        <v>2.98770034400021</v>
+      <c r="B61" t="s">
+        <v>6</v>
       </c>
       <c r="C61">
-        <v>3.66004455390527</v>
-      </c>
-      <c r="D61">
-        <v>5.82997965476049</v>
+        <v>2.022682177849</v>
+      </c>
+      <c r="D61" t="s">
+        <v>6</v>
       </c>
       <c r="E61">
-        <v>3.3872510957889</v>
-      </c>
-      <c r="F61">
-        <v>3.0860039639124</v>
+        <v>2.08168460597163</v>
+      </c>
+      <c r="F61" t="s">
+        <v>6</v>
       </c>
       <c r="G61">
-        <v>4.30020783832701</v>
+        <v>1.4424492597818</v>
       </c>
     </row>
     <row r="62" spans="1:7">
       <c r="A62" s="2">
         <v>33603</v>
       </c>
-      <c r="B62">
-        <v>3.04399898517456</v>
+      <c r="B62" t="s">
+        <v>6</v>
       </c>
       <c r="C62">
-        <v>3.72858888406852</v>
-      </c>
-      <c r="D62">
-        <v>5.34295051130973</v>
+        <v>1.99482983738275</v>
+      </c>
+      <c r="D62" t="s">
+        <v>6</v>
       </c>
       <c r="E62">
-        <v>3.21457605064995</v>
-      </c>
-      <c r="F62">
-        <v>2.18121816530069</v>
+        <v>2.01219645840073</v>
+      </c>
+      <c r="F62" t="s">
+        <v>6</v>
       </c>
       <c r="G62">
-        <v>4.95564161046175</v>
+        <v>1.65540944996808</v>
       </c>
     </row>
     <row r="63" spans="1:7">
       <c r="A63" s="2">
         <v>33694</v>
       </c>
-      <c r="B63">
-        <v>3.53432084870494</v>
+      <c r="B63" t="s">
+        <v>6</v>
       </c>
       <c r="C63">
-        <v>2.82482764647825</v>
-      </c>
-      <c r="D63">
-        <v>6.21340992724748</v>
+        <v>1.8203097532627</v>
+      </c>
+      <c r="D63" t="s">
+        <v>6</v>
       </c>
       <c r="E63">
-        <v>2.19339279662586</v>
-      </c>
-      <c r="F63">
-        <v>3.05220958240564</v>
+        <v>1.55737785131247</v>
+      </c>
+      <c r="F63" t="s">
+        <v>6</v>
       </c>
       <c r="G63">
-        <v>5.0614855138345</v>
+        <v>1.48683673402027</v>
       </c>
     </row>
     <row r="64" spans="1:7">
       <c r="A64" s="2">
         <v>33785</v>
       </c>
-      <c r="B64">
-        <v>2.49359292932832</v>
+      <c r="B64" t="s">
+        <v>6</v>
       </c>
       <c r="C64">
-        <v>1.7499024079708</v>
-      </c>
-      <c r="D64">
-        <v>6.98212621464716</v>
+        <v>2.09510121722401</v>
+      </c>
+      <c r="D64" t="s">
+        <v>6</v>
       </c>
       <c r="E64">
-        <v>2.42765533086317</v>
-      </c>
-      <c r="F64">
-        <v>2.68656904150137</v>
+        <v>1.65605766553507</v>
+      </c>
+      <c r="F64" t="s">
+        <v>6</v>
       </c>
       <c r="G64">
-        <v>5.29403005709569</v>
+        <v>1.51223469195643</v>
       </c>
     </row>
     <row r="65" spans="1:7">
       <c r="A65" s="2">
         <v>33877</v>
       </c>
-      <c r="B65">
-        <v>2.51530253904376</v>
+      <c r="B65" t="s">
+        <v>6</v>
       </c>
       <c r="C65">
-        <v>3.25401774073406</v>
-      </c>
-      <c r="D65">
-        <v>6.85358269606373</v>
+        <v>2.0977770726075</v>
+      </c>
+      <c r="D65" t="s">
+        <v>6</v>
       </c>
       <c r="E65">
-        <v>2.99255548938637</v>
+        <v>1.55738545315089</v>
       </c>
       <c r="F65">
-        <v>3.48189985846007</v>
+        <v>4.57738964217179</v>
       </c>
       <c r="G65">
-        <v>5.36607531977917</v>
+        <v>1.72064671713457</v>
       </c>
     </row>
     <row r="66" spans="1:7">
@@ -1898,22 +1901,22 @@
         <v>33969</v>
       </c>
       <c r="B66">
-        <v>3.08691829137816</v>
+        <v>11.5287886640382</v>
       </c>
       <c r="C66">
-        <v>3.61861778269759</v>
-      </c>
-      <c r="D66">
-        <v>5.54972733325983</v>
+        <v>2.16492209281979</v>
+      </c>
+      <c r="D66" t="s">
+        <v>6</v>
       </c>
       <c r="E66">
-        <v>3.12787136328451</v>
+        <v>1.69547393837798</v>
       </c>
       <c r="F66">
-        <v>3.21728789108452</v>
+        <v>4.46995957492791</v>
       </c>
       <c r="G66">
-        <v>5.51922564196356</v>
+        <v>1.48765761606071</v>
       </c>
     </row>
     <row r="67" spans="1:7">
@@ -1921,22 +1924,22 @@
         <v>34059</v>
       </c>
       <c r="B67">
-        <v>2.75968685199631</v>
+        <v>11.7778930982114</v>
       </c>
       <c r="C67">
-        <v>4.01920479598376</v>
-      </c>
-      <c r="D67">
-        <v>6.00132949218536</v>
+        <v>2.07119785776059</v>
+      </c>
+      <c r="D67" t="s">
+        <v>6</v>
       </c>
       <c r="E67">
-        <v>2.86590187817795</v>
+        <v>1.67002759642413</v>
       </c>
       <c r="F67">
-        <v>3.25964173003846</v>
+        <v>4.30468255210434</v>
       </c>
       <c r="G67">
-        <v>5.85564269833926</v>
+        <v>1.5988831627388</v>
       </c>
     </row>
     <row r="68" spans="1:7">
@@ -1944,22 +1947,22 @@
         <v>34150</v>
       </c>
       <c r="B68">
-        <v>3.18006373377955</v>
+        <v>10.8267815612939</v>
       </c>
       <c r="C68">
-        <v>3.45185851719332</v>
-      </c>
-      <c r="D68">
-        <v>6.44880119996401</v>
+        <v>2.09986117005428</v>
+      </c>
+      <c r="D68" t="s">
+        <v>6</v>
       </c>
       <c r="E68">
-        <v>3.84947067564667</v>
+        <v>1.55829355655309</v>
       </c>
       <c r="F68">
-        <v>2.63915475479053</v>
+        <v>4.22422577651434</v>
       </c>
       <c r="G68">
-        <v>4.6159073636757</v>
+        <v>1.64726999880366</v>
       </c>
     </row>
     <row r="69" spans="1:7">
@@ -1967,22 +1970,22 @@
         <v>34242</v>
       </c>
       <c r="B69">
-        <v>3.70678423954968</v>
+        <v>11.892746879051</v>
       </c>
       <c r="C69">
-        <v>2.91096150750086</v>
-      </c>
-      <c r="D69">
-        <v>5.60888723820168</v>
+        <v>2.0399553966449</v>
+      </c>
+      <c r="D69" t="s">
+        <v>6</v>
       </c>
       <c r="E69">
-        <v>2.88589232218114</v>
+        <v>1.80427392074445</v>
       </c>
       <c r="F69">
-        <v>3.52550897612159</v>
+        <v>4.15362520979287</v>
       </c>
       <c r="G69">
-        <v>4.38668319597947</v>
+        <v>1.64676793523884</v>
       </c>
     </row>
     <row r="70" spans="1:7">
@@ -1990,22 +1993,22 @@
         <v>34334</v>
       </c>
       <c r="B70">
-        <v>4.24485415287031</v>
+        <v>10.9761273483446</v>
       </c>
       <c r="C70">
-        <v>3.15358349471062</v>
-      </c>
-      <c r="D70">
-        <v>6.0293701842964</v>
+        <v>1.87903837539082</v>
+      </c>
+      <c r="D70" t="s">
+        <v>6</v>
       </c>
       <c r="E70">
-        <v>3.58396779198549</v>
+        <v>1.83805383298353</v>
       </c>
       <c r="F70">
-        <v>3.7505489707861</v>
+        <v>4.31640649562166</v>
       </c>
       <c r="G70">
-        <v>4.02513146675943</v>
+        <v>1.67291929919607</v>
       </c>
     </row>
     <row r="71" spans="1:7">
@@ -2013,22 +2016,22 @@
         <v>34424</v>
       </c>
       <c r="B71">
-        <v>3.44462124068157</v>
+        <v>11.5601015089337</v>
       </c>
       <c r="C71">
-        <v>2.38062899060466</v>
-      </c>
-      <c r="D71">
-        <v>4.8998103953338</v>
+        <v>2.22815212384251</v>
+      </c>
+      <c r="D71" t="s">
+        <v>6</v>
       </c>
       <c r="E71">
-        <v>2.92040247018351</v>
+        <v>1.85375835980534</v>
       </c>
       <c r="F71">
-        <v>3.13253979740478</v>
+        <v>4.3536615409008</v>
       </c>
       <c r="G71">
-        <v>5.06735461093824</v>
+        <v>1.67913701081313</v>
       </c>
     </row>
     <row r="72" spans="1:7">
@@ -2036,22 +2039,22 @@
         <v>34515</v>
       </c>
       <c r="B72">
-        <v>4.63170624185528</v>
+        <v>11.0537700169304</v>
       </c>
       <c r="C72">
-        <v>3.2967795129626</v>
-      </c>
-      <c r="D72">
-        <v>4.80955167490866</v>
+        <v>1.99941020764081</v>
+      </c>
+      <c r="D72" t="s">
+        <v>6</v>
       </c>
       <c r="E72">
-        <v>2.88640826357412</v>
+        <v>1.71719732932451</v>
       </c>
       <c r="F72">
-        <v>3.51093665478122</v>
+        <v>4.31253667073899</v>
       </c>
       <c r="G72">
-        <v>4.58947849875069</v>
+        <v>1.732377290737</v>
       </c>
     </row>
     <row r="73" spans="1:7">
@@ -2059,22 +2062,22 @@
         <v>34607</v>
       </c>
       <c r="B73">
-        <v>6.46185830242184</v>
+        <v>11.0113776346716</v>
       </c>
       <c r="C73">
-        <v>3.51746127599607</v>
-      </c>
-      <c r="D73">
-        <v>3.92111903277024</v>
+        <v>2.20655668430014</v>
+      </c>
+      <c r="D73" t="s">
+        <v>6</v>
       </c>
       <c r="E73">
-        <v>2.80920607579392</v>
+        <v>1.70620818351909</v>
       </c>
       <c r="F73">
-        <v>2.74353876501279</v>
+        <v>4.12752970351382</v>
       </c>
       <c r="G73">
-        <v>3.35389792957918</v>
+        <v>1.8386248532624</v>
       </c>
     </row>
     <row r="74" spans="1:7">
@@ -2082,22 +2085,22 @@
         <v>34699</v>
       </c>
       <c r="B74">
-        <v>6.22324051734662</v>
+        <v>11.259749752508</v>
       </c>
       <c r="C74">
-        <v>3.35088019255309</v>
-      </c>
-      <c r="D74">
-        <v>5.30333086906888</v>
+        <v>2.22558930105066</v>
+      </c>
+      <c r="D74" t="s">
+        <v>6</v>
       </c>
       <c r="E74">
-        <v>3.90069217022352</v>
+        <v>1.76677550395354</v>
       </c>
       <c r="F74">
-        <v>3.29500044270197</v>
+        <v>4.3140414599315</v>
       </c>
       <c r="G74">
-        <v>2.84444923981012</v>
+        <v>1.6637372426285</v>
       </c>
     </row>
     <row r="75" spans="1:7">
@@ -2105,22 +2108,22 @@
         <v>34789</v>
       </c>
       <c r="B75">
-        <v>6.05635149993626</v>
+        <v>12.1879886231342</v>
       </c>
       <c r="C75">
-        <v>3.02628385559444</v>
-      </c>
-      <c r="D75">
-        <v>5.69325436407677</v>
+        <v>2.10838631948545</v>
+      </c>
+      <c r="D75" t="s">
+        <v>6</v>
       </c>
       <c r="E75">
-        <v>3.06816884724886</v>
+        <v>1.77469639825652</v>
       </c>
       <c r="F75">
-        <v>3.13463523258226</v>
+        <v>4.30204398587884</v>
       </c>
       <c r="G75">
-        <v>4.50479858583286</v>
+        <v>1.81154608068028</v>
       </c>
     </row>
     <row r="76" spans="1:7">
@@ -2128,22 +2131,22 @@
         <v>34880</v>
       </c>
       <c r="B76">
-        <v>5.19256153564615</v>
+        <v>11.9194366898497</v>
       </c>
       <c r="C76">
-        <v>3.80230719111436</v>
-      </c>
-      <c r="D76">
-        <v>4.75731085710412</v>
+        <v>2.14840220224225</v>
+      </c>
+      <c r="D76" t="s">
+        <v>6</v>
       </c>
       <c r="E76">
-        <v>2.26219264200957</v>
+        <v>1.75280396454217</v>
       </c>
       <c r="F76">
-        <v>3.93748631162369</v>
+        <v>4.32490178671283</v>
       </c>
       <c r="G76">
-        <v>2.49406764836276</v>
+        <v>1.90282325904089</v>
       </c>
     </row>
     <row r="77" spans="1:7">
@@ -2151,22 +2154,22 @@
         <v>34972</v>
       </c>
       <c r="B77">
-        <v>8.1093354399863</v>
+        <v>12.0993639289455</v>
       </c>
       <c r="C77">
-        <v>3.38930467066655</v>
-      </c>
-      <c r="D77">
-        <v>5.82211272444963</v>
+        <v>2.07329127287386</v>
+      </c>
+      <c r="D77" t="s">
+        <v>6</v>
       </c>
       <c r="E77">
-        <v>2.91779996289241</v>
+        <v>1.64511620020381</v>
       </c>
       <c r="F77">
-        <v>3.67499018283036</v>
+        <v>4.44117522818505</v>
       </c>
       <c r="G77">
-        <v>4.72210169784869</v>
+        <v>1.8296069709296</v>
       </c>
     </row>
     <row r="78" spans="1:7">
@@ -2174,22 +2177,22 @@
         <v>35064</v>
       </c>
       <c r="B78">
-        <v>5.18053320758383</v>
+        <v>11.1009542479852</v>
       </c>
       <c r="C78">
-        <v>4.19020934444559</v>
-      </c>
-      <c r="D78">
-        <v>3.90570618134532</v>
+        <v>2.04544214196154</v>
+      </c>
+      <c r="D78" t="s">
+        <v>6</v>
       </c>
       <c r="E78">
-        <v>3.26320594663869</v>
+        <v>1.69427616259219</v>
       </c>
       <c r="F78">
-        <v>3.79749176166345</v>
+        <v>4.39707276919767</v>
       </c>
       <c r="G78">
-        <v>5.64924752873094</v>
+        <v>1.7092364756149</v>
       </c>
     </row>
     <row r="79" spans="1:7">
@@ -2197,22 +2200,22 @@
         <v>35155</v>
       </c>
       <c r="B79">
-        <v>6.82940606987712</v>
+        <v>10.9209313574545</v>
       </c>
       <c r="C79">
-        <v>3.5242946696036</v>
-      </c>
-      <c r="D79">
-        <v>4.8260135189438</v>
+        <v>1.9571668329707</v>
+      </c>
+      <c r="D79" t="s">
+        <v>6</v>
       </c>
       <c r="E79">
-        <v>2.91424495807807</v>
+        <v>1.7716049132034</v>
       </c>
       <c r="F79">
-        <v>3.1911188419019</v>
+        <v>4.13772613412988</v>
       </c>
       <c r="G79">
-        <v>5.14470045107241</v>
+        <v>1.59834847130169</v>
       </c>
     </row>
     <row r="80" spans="1:7">
@@ -2220,22 +2223,22 @@
         <v>35246</v>
       </c>
       <c r="B80">
-        <v>7.60318377720985</v>
+        <v>11.3648924542997</v>
       </c>
       <c r="C80">
-        <v>2.528894009677</v>
-      </c>
-      <c r="D80">
-        <v>4.54632313469486</v>
+        <v>2.13275451235846</v>
+      </c>
+      <c r="D80" t="s">
+        <v>6</v>
       </c>
       <c r="E80">
-        <v>3.26747195086403</v>
+        <v>1.67484719740393</v>
       </c>
       <c r="F80">
-        <v>3.41236596700834</v>
+        <v>4.29417043951677</v>
       </c>
       <c r="G80">
-        <v>4.00201152578946</v>
+        <v>1.76189874687264</v>
       </c>
     </row>
     <row r="81" spans="1:7">
@@ -2243,22 +2246,22 @@
         <v>35338</v>
       </c>
       <c r="B81">
-        <v>6.62537242397733</v>
+        <v>11.632833546493</v>
       </c>
       <c r="C81">
-        <v>3.51100755678623</v>
-      </c>
-      <c r="D81">
-        <v>5.28323079808794</v>
+        <v>2.08052381658844</v>
+      </c>
+      <c r="D81" t="s">
+        <v>6</v>
       </c>
       <c r="E81">
-        <v>3.16716664567513</v>
+        <v>1.68797682748167</v>
       </c>
       <c r="F81">
-        <v>2.83344485764027</v>
+        <v>4.46415529116685</v>
       </c>
       <c r="G81">
-        <v>4.68966251579691</v>
+        <v>1.84701610429225</v>
       </c>
     </row>
     <row r="82" spans="1:7">
@@ -2266,22 +2269,22 @@
         <v>35430</v>
       </c>
       <c r="B82">
-        <v>5.69993539564178</v>
+        <v>11.2501637888046</v>
       </c>
       <c r="C82">
-        <v>3.24221579547631</v>
-      </c>
-      <c r="D82">
-        <v>4.08629650647042</v>
+        <v>2.15986651137765</v>
+      </c>
+      <c r="D82" t="s">
+        <v>6</v>
       </c>
       <c r="E82">
-        <v>2.60088064337447</v>
+        <v>1.73183708763831</v>
       </c>
       <c r="F82">
-        <v>3.33011041798582</v>
+        <v>4.31757813640296</v>
       </c>
       <c r="G82">
-        <v>4.47990931311491</v>
+        <v>1.72901722484497</v>
       </c>
     </row>
     <row r="83" spans="1:7">
@@ -2289,22 +2292,22 @@
         <v>35520</v>
       </c>
       <c r="B83">
-        <v>6.93316482493845</v>
+        <v>11.681304713473</v>
       </c>
       <c r="C83">
-        <v>2.99100288272361</v>
-      </c>
-      <c r="D83">
-        <v>5.0070218404115</v>
+        <v>2.11632461037672</v>
+      </c>
+      <c r="D83" t="s">
+        <v>6</v>
       </c>
       <c r="E83">
-        <v>3.03453091489444</v>
+        <v>1.80144369178388</v>
       </c>
       <c r="F83">
-        <v>3.26592304496372</v>
+        <v>4.45912921334698</v>
       </c>
       <c r="G83">
-        <v>4.73047639159998</v>
+        <v>1.73497939516125</v>
       </c>
     </row>
     <row r="84" spans="1:7">
@@ -2312,22 +2315,22 @@
         <v>35611</v>
       </c>
       <c r="B84">
-        <v>6.89541538839334</v>
+        <v>11.9089085792888</v>
       </c>
       <c r="C84">
-        <v>3.69262252066495</v>
-      </c>
-      <c r="D84">
-        <v>6.55997480471942</v>
+        <v>2.12280126987739</v>
+      </c>
+      <c r="D84" t="s">
+        <v>6</v>
       </c>
       <c r="E84">
-        <v>3.59477708840818</v>
+        <v>1.63795855569194</v>
       </c>
       <c r="F84">
-        <v>3.07534103552206</v>
+        <v>4.34603642814309</v>
       </c>
       <c r="G84">
-        <v>4.66875779766959</v>
+        <v>1.8944798563742</v>
       </c>
     </row>
     <row r="85" spans="1:7">
@@ -2335,22 +2338,22 @@
         <v>35703</v>
       </c>
       <c r="B85">
-        <v>6.06499332945784</v>
+        <v>10.2492749362792</v>
       </c>
       <c r="C85">
-        <v>3.51739814710113</v>
-      </c>
-      <c r="D85">
-        <v>5.1389041905861</v>
+        <v>2.02102480489402</v>
+      </c>
+      <c r="D85" t="s">
+        <v>6</v>
       </c>
       <c r="E85">
-        <v>3.71818487391408</v>
+        <v>2.01594814912595</v>
       </c>
       <c r="F85">
-        <v>4.23488210070698</v>
+        <v>4.0528172336614</v>
       </c>
       <c r="G85">
-        <v>5.17382648530404</v>
+        <v>1.61272401463621</v>
       </c>
     </row>
     <row r="86" spans="1:7">
@@ -2358,22 +2361,22 @@
         <v>35795</v>
       </c>
       <c r="B86">
-        <v>7.94567262105315</v>
+        <v>11.1623889527242</v>
       </c>
       <c r="C86">
-        <v>3.37449569828132</v>
-      </c>
-      <c r="D86">
-        <v>4.29092976819949</v>
+        <v>2.18436137343957</v>
+      </c>
+      <c r="D86" t="s">
+        <v>6</v>
       </c>
       <c r="E86">
-        <v>2.39948318417348</v>
+        <v>1.80491846755661</v>
       </c>
       <c r="F86">
-        <v>4.77017001769071</v>
+        <v>4.46838493299522</v>
       </c>
       <c r="G86">
-        <v>4.34814941857483</v>
+        <v>1.73681216684153</v>
       </c>
     </row>
     <row r="87" spans="1:7">
@@ -2381,22 +2384,22 @@
         <v>35885</v>
       </c>
       <c r="B87">
-        <v>8.97600749784096</v>
+        <v>11.6025486187836</v>
       </c>
       <c r="C87">
-        <v>3.52776751192682</v>
-      </c>
-      <c r="D87">
-        <v>4.53427257640591</v>
+        <v>2.13169306641018</v>
+      </c>
+      <c r="D87" t="s">
+        <v>6</v>
       </c>
       <c r="E87">
-        <v>3.2355391566724</v>
+        <v>1.81779464705566</v>
       </c>
       <c r="F87">
-        <v>2.83328700962839</v>
+        <v>4.41256949087452</v>
       </c>
       <c r="G87">
-        <v>5.32923710547141</v>
+        <v>1.84353436331551</v>
       </c>
     </row>
     <row r="88" spans="1:7">
@@ -2404,22 +2407,22 @@
         <v>35976</v>
       </c>
       <c r="B88">
-        <v>7.08006709020241</v>
+        <v>11.3728176531443</v>
       </c>
       <c r="C88">
-        <v>2.97857229702653</v>
-      </c>
-      <c r="D88">
-        <v>4.53505572073219</v>
+        <v>2.05649454414789</v>
+      </c>
+      <c r="D88" t="s">
+        <v>6</v>
       </c>
       <c r="E88">
-        <v>2.20123977286196</v>
+        <v>1.76167103212474</v>
       </c>
       <c r="F88">
-        <v>3.80863045804367</v>
+        <v>4.19148789546974</v>
       </c>
       <c r="G88">
-        <v>4.13138086423934</v>
+        <v>1.80225308982679</v>
       </c>
     </row>
     <row r="89" spans="1:7">
@@ -2427,22 +2430,22 @@
         <v>36068</v>
       </c>
       <c r="B89">
-        <v>7.77120309342833</v>
+        <v>11.2371946572866</v>
       </c>
       <c r="C89">
-        <v>4.28384829668898</v>
-      </c>
-      <c r="D89">
-        <v>5.30879275584626</v>
+        <v>2.14118884952351</v>
+      </c>
+      <c r="D89" t="s">
+        <v>6</v>
       </c>
       <c r="E89">
-        <v>2.60996843399897</v>
+        <v>1.71484545863738</v>
       </c>
       <c r="F89">
-        <v>3.03111563128184</v>
+        <v>4.27759053155186</v>
       </c>
       <c r="G89">
-        <v>3.24915322969918</v>
+        <v>2.05845320466328</v>
       </c>
     </row>
     <row r="90" spans="1:7">
@@ -2450,22 +2453,22 @@
         <v>36160</v>
       </c>
       <c r="B90">
-        <v>7.48406393285918</v>
+        <v>10.940160984094</v>
       </c>
       <c r="C90">
-        <v>3.13508045525458</v>
-      </c>
-      <c r="D90">
-        <v>5.24670943612355</v>
+        <v>2.05340807733272</v>
+      </c>
+      <c r="D90" t="s">
+        <v>6</v>
       </c>
       <c r="E90">
-        <v>2.73597621932486</v>
+        <v>1.70009895947352</v>
       </c>
       <c r="F90">
-        <v>3.33308690569817</v>
+        <v>4.23548669376991</v>
       </c>
       <c r="G90">
-        <v>4.62537546001284</v>
+        <v>2.0527009467375</v>
       </c>
     </row>
     <row r="91" spans="1:7">
@@ -2473,22 +2476,22 @@
         <v>36250</v>
       </c>
       <c r="B91">
-        <v>7.29982413983715</v>
+        <v>11.35661678325</v>
       </c>
       <c r="C91">
-        <v>2.5855343129683</v>
-      </c>
-      <c r="D91">
-        <v>4.98578068019953</v>
+        <v>2.06782626111272</v>
+      </c>
+      <c r="D91" t="s">
+        <v>6</v>
       </c>
       <c r="E91">
-        <v>3.96910435110209</v>
+        <v>1.61678320686847</v>
       </c>
       <c r="F91">
-        <v>3.48489082167429</v>
+        <v>4.5820566430342</v>
       </c>
       <c r="G91">
-        <v>4.20248604866776</v>
+        <v>2.17525282811972</v>
       </c>
     </row>
     <row r="92" spans="1:7">
@@ -2496,22 +2499,22 @@
         <v>36341</v>
       </c>
       <c r="B92">
-        <v>8.02424743655727</v>
+        <v>10.7101381621002</v>
       </c>
       <c r="C92">
-        <v>2.71799583907464</v>
-      </c>
-      <c r="D92">
-        <v>5.886656547192</v>
+        <v>2.1232711101824</v>
+      </c>
+      <c r="D92" t="s">
+        <v>6</v>
       </c>
       <c r="E92">
-        <v>2.96285721720899</v>
+        <v>1.54636396615088</v>
       </c>
       <c r="F92">
-        <v>3.1684237877434</v>
+        <v>4.37675390458355</v>
       </c>
       <c r="G92">
-        <v>4.84496926010554</v>
+        <v>2.65027743504966</v>
       </c>
     </row>
     <row r="93" spans="1:7">
@@ -2519,22 +2522,22 @@
         <v>36433</v>
       </c>
       <c r="B93">
-        <v>7.98348577563898</v>
-      </c>
-      <c r="C93">
-        <v>3.56793880989666</v>
-      </c>
-      <c r="D93">
-        <v>6.01602117619248</v>
+        <v>10.2448406091271</v>
+      </c>
+      <c r="C93" t="s">
+        <v>6</v>
+      </c>
+      <c r="D93" t="s">
+        <v>6</v>
       </c>
       <c r="E93">
-        <v>3.65914202830935</v>
+        <v>1.37640873770761</v>
       </c>
       <c r="F93">
-        <v>2.73180790786539</v>
+        <v>3.90226456574857</v>
       </c>
       <c r="G93">
-        <v>4.59700210936487</v>
+        <v>1.31947341392965</v>
       </c>
     </row>
     <row r="94" spans="1:7">
@@ -2542,22 +2545,22 @@
         <v>36525</v>
       </c>
       <c r="B94">
-        <v>7.01074698894931</v>
-      </c>
-      <c r="C94">
-        <v>3.35879165439202</v>
-      </c>
-      <c r="D94">
-        <v>4.85018995208546</v>
+        <v>10.1094973663262</v>
+      </c>
+      <c r="C94" t="s">
+        <v>6</v>
+      </c>
+      <c r="D94" t="s">
+        <v>6</v>
       </c>
       <c r="E94">
-        <v>3.67139720659269</v>
+        <v>1.4489446352224</v>
       </c>
       <c r="F94">
-        <v>3.36013965723564</v>
+        <v>4.02696579772927</v>
       </c>
       <c r="G94">
-        <v>3.98354087242579</v>
+        <v>1.54899109379374</v>
       </c>
     </row>
     <row r="95" spans="1:7">
@@ -2565,22 +2568,22 @@
         <v>36616</v>
       </c>
       <c r="B95">
-        <v>10.0178002450969</v>
-      </c>
-      <c r="C95">
-        <v>3.41197120587846</v>
-      </c>
-      <c r="D95">
-        <v>5.43898230366075</v>
+        <v>8.78900078696012</v>
+      </c>
+      <c r="C95" t="s">
+        <v>6</v>
+      </c>
+      <c r="D95" t="s">
+        <v>6</v>
       </c>
       <c r="E95">
-        <v>3.58321394731296</v>
+        <v>1.48753703288571</v>
       </c>
       <c r="F95">
-        <v>3.03951355786298</v>
+        <v>3.59300166593503</v>
       </c>
       <c r="G95">
-        <v>3.98930270174933</v>
+        <v>1.31771980936444</v>
       </c>
     </row>
     <row r="96" spans="1:7">
@@ -2588,22 +2591,22 @@
         <v>36707</v>
       </c>
       <c r="B96">
-        <v>9.49287805165462</v>
-      </c>
-      <c r="C96">
-        <v>4.02591587027826</v>
-      </c>
-      <c r="D96">
-        <v>4.35169841349298</v>
+        <v>8.83275382577617</v>
+      </c>
+      <c r="C96" t="s">
+        <v>6</v>
+      </c>
+      <c r="D96" t="s">
+        <v>6</v>
       </c>
       <c r="E96">
-        <v>3.54004964705399</v>
+        <v>1.17140631003719</v>
       </c>
       <c r="F96">
-        <v>2.75325481227366</v>
+        <v>4.08851156344686</v>
       </c>
       <c r="G96">
-        <v>3.49080264890074</v>
+        <v>1.92516436132976</v>
       </c>
     </row>
     <row r="97" spans="1:7">
@@ -2611,22 +2614,22 @@
         <v>36799</v>
       </c>
       <c r="B97">
-        <v>7.11477265094643</v>
-      </c>
-      <c r="C97">
-        <v>2.8933831170323</v>
-      </c>
-      <c r="D97">
-        <v>4.21444024070812</v>
+        <v>9.36690552481202</v>
+      </c>
+      <c r="C97" t="s">
+        <v>6</v>
+      </c>
+      <c r="D97" t="s">
+        <v>6</v>
       </c>
       <c r="E97">
-        <v>3.8876550747385</v>
+        <v>1.58934286082947</v>
       </c>
       <c r="F97">
-        <v>3.39355213305862</v>
+        <v>3.92343602278146</v>
       </c>
       <c r="G97">
-        <v>5.02686341355713</v>
+        <v>1.20683539857227</v>
       </c>
     </row>
     <row r="98" spans="1:7">
@@ -2634,22 +2637,22 @@
         <v>36891</v>
       </c>
       <c r="B98">
-        <v>9.87704220359008</v>
-      </c>
-      <c r="C98">
-        <v>3.29250581272948</v>
-      </c>
-      <c r="D98">
-        <v>5.12637767096151</v>
+        <v>9.89877573777548</v>
+      </c>
+      <c r="C98" t="s">
+        <v>6</v>
+      </c>
+      <c r="D98" t="s">
+        <v>6</v>
       </c>
       <c r="E98">
-        <v>3.20386406658173</v>
+        <v>1.39595809019105</v>
       </c>
       <c r="F98">
-        <v>3.23373157827007</v>
+        <v>5.73525118008016</v>
       </c>
       <c r="G98">
-        <v>4.18139173875466</v>
+        <v>1.23991734164424</v>
       </c>
     </row>
     <row r="99" spans="1:7">
@@ -2657,22 +2660,22 @@
         <v>36981</v>
       </c>
       <c r="B99">
-        <v>7.54959305023913</v>
+        <v>14.4997592712862</v>
       </c>
       <c r="C99">
-        <v>3.20258294677492</v>
+        <v>2.42431493695005</v>
       </c>
       <c r="D99">
-        <v>4.42761422854696</v>
+        <v>2.42629463778129</v>
       </c>
       <c r="E99">
-        <v>3.49094234764634</v>
+        <v>2.85629591623684</v>
       </c>
       <c r="F99">
-        <v>2.80651556677533</v>
+        <v>3.56603196159375</v>
       </c>
       <c r="G99">
-        <v>4.02702719415588</v>
+        <v>1.93258786455489</v>
       </c>
     </row>
     <row r="100" spans="1:7">
@@ -2680,22 +2683,22 @@
         <v>37072</v>
       </c>
       <c r="B100">
-        <v>6.65398688830158</v>
+        <v>14.5338612247089</v>
       </c>
       <c r="C100">
-        <v>2.74328324818311</v>
+        <v>2.42134283345568</v>
       </c>
       <c r="D100">
-        <v>4.13292543782541</v>
+        <v>2.42177099501459</v>
       </c>
       <c r="E100">
-        <v>2.80084754829016</v>
+        <v>2.85341316357879</v>
       </c>
       <c r="F100">
-        <v>3.86830661430694</v>
+        <v>3.55793752893338</v>
       </c>
       <c r="G100">
-        <v>3.59117372875894</v>
+        <v>1.9368814766736</v>
       </c>
     </row>
     <row r="101" spans="1:7">
@@ -2703,22 +2706,22 @@
         <v>37164</v>
       </c>
       <c r="B101">
-        <v>5.31549434679443</v>
+        <v>14.5134750285093</v>
       </c>
       <c r="C101">
-        <v>3.24012352822325</v>
+        <v>2.42212740707187</v>
       </c>
       <c r="D101">
-        <v>4.7209127977256</v>
+        <v>2.42950919849146</v>
       </c>
       <c r="E101">
-        <v>3.55302703809798</v>
+        <v>2.85504989551163</v>
       </c>
       <c r="F101">
-        <v>3.20516754605088</v>
+        <v>3.55578562921686</v>
       </c>
       <c r="G101">
-        <v>4.61021811439523</v>
+        <v>1.93727611780723</v>
       </c>
     </row>
     <row r="102" spans="1:7">
@@ -2726,22 +2729,22 @@
         <v>37256</v>
       </c>
       <c r="B102">
-        <v>6.7427734926202</v>
+        <v>14.4970269953257</v>
       </c>
       <c r="C102">
-        <v>3.26471039340388</v>
+        <v>2.42507349270551</v>
       </c>
       <c r="D102">
-        <v>4.54939690900019</v>
+        <v>2.4233756801888</v>
       </c>
       <c r="E102">
-        <v>3.16249566362091</v>
+        <v>2.85009762336441</v>
       </c>
       <c r="F102">
-        <v>3.50663921808226</v>
+        <v>3.55938256696277</v>
       </c>
       <c r="G102">
-        <v>4.60532635819248</v>
+        <v>1.93401359430737</v>
       </c>
     </row>
     <row r="103" spans="1:7">
@@ -2749,22 +2752,22 @@
         <v>37346</v>
       </c>
       <c r="B103">
-        <v>7.79766426073341</v>
+        <v>14.4968131780586</v>
       </c>
       <c r="C103">
-        <v>3.13740613813288</v>
+        <v>2.42241186164098</v>
       </c>
       <c r="D103">
-        <v>3.96093348373505</v>
+        <v>2.42463809649748</v>
       </c>
       <c r="E103">
-        <v>3.00848391863652</v>
+        <v>2.8546334016012</v>
       </c>
       <c r="F103">
-        <v>4.12460162173226</v>
+        <v>3.56191009960268</v>
       </c>
       <c r="G103">
-        <v>4.63504453006624</v>
+        <v>1.93635148355854</v>
       </c>
     </row>
     <row r="104" spans="1:7">
@@ -2772,22 +2775,22 @@
         <v>37437</v>
       </c>
       <c r="B104">
-        <v>6.3343688881829</v>
+        <v>11.3605616136183</v>
       </c>
       <c r="C104">
-        <v>2.29090237757353</v>
+        <v>4.7890603026644</v>
       </c>
       <c r="D104">
-        <v>4.922392971111</v>
+        <v>4.89193737061193</v>
       </c>
       <c r="E104">
-        <v>4.47435084772614</v>
+        <v>1.81430896850551</v>
       </c>
       <c r="F104">
-        <v>2.78362891113436</v>
+        <v>4.38727735915223</v>
       </c>
       <c r="G104">
-        <v>4.37627654436718</v>
+        <v>1.45835633356527</v>
       </c>
     </row>
     <row r="105" spans="1:7">
@@ -2795,22 +2798,22 @@
         <v>37529</v>
       </c>
       <c r="B105">
-        <v>7.98382635445778</v>
+        <v>14.640134245246</v>
       </c>
       <c r="C105">
-        <v>2.7044795938161</v>
+        <v>2.3566931216303</v>
       </c>
       <c r="D105">
-        <v>3.72291571112493</v>
+        <v>2.35161526003112</v>
       </c>
       <c r="E105">
-        <v>3.74649610058354</v>
+        <v>2.96948120343982</v>
       </c>
       <c r="F105">
-        <v>1.7182104384262</v>
+        <v>3.07446703478623</v>
       </c>
       <c r="G105">
-        <v>3.28139036760204</v>
+        <v>1.971520627749</v>
       </c>
     </row>
     <row r="106" spans="1:7">
@@ -2818,22 +2821,22 @@
         <v>37621</v>
       </c>
       <c r="B106">
-        <v>7.5890990914324</v>
+        <v>14.6491540608426</v>
       </c>
       <c r="C106">
-        <v>3.04266673280528</v>
+        <v>2.35404233784626</v>
       </c>
       <c r="D106">
-        <v>4.03050550838286</v>
+        <v>2.35131768369427</v>
       </c>
       <c r="E106">
-        <v>3.74752165033294</v>
+        <v>2.96141652304554</v>
       </c>
       <c r="F106">
-        <v>3.56151330723987</v>
+        <v>3.07120371815901</v>
       </c>
       <c r="G106">
-        <v>4.07512991994333</v>
+        <v>1.96622349059934</v>
       </c>
     </row>
     <row r="107" spans="1:7">
@@ -2841,22 +2844,22 @@
         <v>37711</v>
       </c>
       <c r="B107">
-        <v>8.63572042139557</v>
+        <v>14.6498793665767</v>
       </c>
       <c r="C107">
-        <v>2.76873276191226</v>
+        <v>2.35089770250397</v>
       </c>
       <c r="D107">
-        <v>3.99166018237073</v>
+        <v>2.35289426495139</v>
       </c>
       <c r="E107">
-        <v>3.34833041744393</v>
+        <v>2.97006801373822</v>
       </c>
       <c r="F107">
-        <v>2.51215091980982</v>
+        <v>3.07131122069152</v>
       </c>
       <c r="G107">
-        <v>5.05003424820356</v>
+        <v>1.96532181200503</v>
       </c>
     </row>
     <row r="108" spans="1:7">
@@ -2864,22 +2867,22 @@
         <v>37802</v>
       </c>
       <c r="B108">
-        <v>8.84344514345505</v>
+        <v>14.852806885949</v>
       </c>
       <c r="C108">
-        <v>2.87381151081</v>
+        <v>2.35372758505535</v>
       </c>
       <c r="D108">
-        <v>4.32013847944306</v>
+        <v>2.35680441753056</v>
       </c>
       <c r="E108">
-        <v>3.58388063995175</v>
+        <v>2.73746911261477</v>
       </c>
       <c r="F108">
-        <v>3.376343049632</v>
+        <v>3.08489783964127</v>
       </c>
       <c r="G108">
-        <v>3.77793649669097</v>
+        <v>1.99293102356688</v>
       </c>
     </row>
     <row r="109" spans="1:7">
@@ -2887,22 +2890,22 @@
         <v>37894</v>
       </c>
       <c r="B109">
-        <v>8.92910760850678</v>
+        <v>14.7323023068848</v>
       </c>
       <c r="C109">
-        <v>3.08246843838385</v>
+        <v>2.35502152034858</v>
       </c>
       <c r="D109">
-        <v>5.59003672170474</v>
+        <v>2.35236139991648</v>
       </c>
       <c r="E109">
-        <v>3.88525332777049</v>
+        <v>2.91346605689084</v>
       </c>
       <c r="F109">
-        <v>2.61614749992531</v>
+        <v>3.0815398361104</v>
       </c>
       <c r="G109">
-        <v>4.64666893972356</v>
+        <v>1.97867023984873</v>
       </c>
     </row>
     <row r="110" spans="1:7">
@@ -2910,22 +2913,22 @@
         <v>37986</v>
       </c>
       <c r="B110">
-        <v>10.4351786049122</v>
+        <v>14.7467815396371</v>
       </c>
       <c r="C110">
-        <v>3.21697152071708</v>
+        <v>2.35691383280285</v>
       </c>
       <c r="D110">
-        <v>6.08081307218767</v>
+        <v>2.3591350015204</v>
       </c>
       <c r="E110">
-        <v>3.6136272307022</v>
+        <v>2.91162678808121</v>
       </c>
       <c r="F110">
-        <v>3.78509395683287</v>
+        <v>3.08487475003934</v>
       </c>
       <c r="G110">
-        <v>4.51530215730714</v>
+        <v>1.98159698000078</v>
       </c>
     </row>
     <row r="111" spans="1:7">
@@ -2933,22 +2936,22 @@
         <v>38077</v>
       </c>
       <c r="B111">
-        <v>9.58802633936698</v>
+        <v>14.7494279858767</v>
       </c>
       <c r="C111">
-        <v>2.49695688282852</v>
+        <v>2.35326519358517</v>
       </c>
       <c r="D111">
-        <v>3.73937065196989</v>
+        <v>2.35779469104854</v>
       </c>
       <c r="E111">
-        <v>4.08659568396015</v>
+        <v>2.91270276168355</v>
       </c>
       <c r="F111">
-        <v>3.73329919348037</v>
+        <v>3.07986065748251</v>
       </c>
       <c r="G111">
-        <v>4.24719220684363</v>
+        <v>1.9846950310936</v>
       </c>
     </row>
     <row r="112" spans="1:7">
@@ -2956,22 +2959,22 @@
         <v>38168</v>
       </c>
       <c r="B112">
-        <v>11.2125766603878</v>
+        <v>14.729538129525</v>
       </c>
       <c r="C112">
-        <v>2.78923058978029</v>
+        <v>2.35932202051652</v>
       </c>
       <c r="D112">
-        <v>3.45114646098298</v>
+        <v>2.35859135760151</v>
       </c>
       <c r="E112">
-        <v>3.10732598911554</v>
+        <v>2.91206332823263</v>
       </c>
       <c r="F112">
-        <v>4.8886696612157</v>
+        <v>3.0856192394826</v>
       </c>
       <c r="G112">
-        <v>3.26947823299915</v>
+        <v>1.98530236829988</v>
       </c>
     </row>
     <row r="113" spans="1:7">
@@ -2979,22 +2982,22 @@
         <v>38260</v>
       </c>
       <c r="B113">
-        <v>12.3431956475009</v>
+        <v>14.7311371121306</v>
       </c>
       <c r="C113">
-        <v>2.5675690001393</v>
+        <v>2.35643640591734</v>
       </c>
       <c r="D113">
-        <v>5.62238032887965</v>
+        <v>2.35690127785625</v>
       </c>
       <c r="E113">
-        <v>2.9334379658654</v>
+        <v>2.91262221958738</v>
       </c>
       <c r="F113">
-        <v>2.7166054710753</v>
+        <v>3.07840135504121</v>
       </c>
       <c r="G113">
-        <v>4.25753144624478</v>
+        <v>2.07277226924206</v>
       </c>
     </row>
     <row r="114" spans="1:7">
@@ -3002,22 +3005,22 @@
         <v>38352</v>
       </c>
       <c r="B114">
-        <v>12.251036449982</v>
+        <v>14.7388384416783</v>
       </c>
       <c r="C114">
-        <v>2.57692494519809</v>
+        <v>2.35476108957518</v>
       </c>
       <c r="D114">
-        <v>4.1242247331485</v>
+        <v>2.35838038466058</v>
       </c>
       <c r="E114">
-        <v>4.29552047875503</v>
+        <v>2.91699838388116</v>
       </c>
       <c r="F114">
-        <v>3.4195792944114</v>
+        <v>3.08595313207097</v>
       </c>
       <c r="G114">
-        <v>3.81003714842421</v>
+        <v>2.06997441277246</v>
       </c>
     </row>
     <row r="115" spans="1:7">
@@ -3025,22 +3028,22 @@
         <v>38442</v>
       </c>
       <c r="B115">
-        <v>11.8431777205685</v>
+        <v>14.7652091820065</v>
       </c>
       <c r="C115">
-        <v>2.187215605401</v>
+        <v>2.3567565158485</v>
       </c>
       <c r="D115">
-        <v>3.57904341628887</v>
+        <v>2.35878954326899</v>
       </c>
       <c r="E115">
-        <v>2.25077549658902</v>
+        <v>2.91620356654759</v>
       </c>
       <c r="F115">
-        <v>4.25492922713384</v>
+        <v>3.08381160272166</v>
       </c>
       <c r="G115">
-        <v>4.27422063064206</v>
+        <v>2.07369254475878</v>
       </c>
     </row>
     <row r="116" spans="1:7">
@@ -3048,22 +3051,22 @@
         <v>38533</v>
       </c>
       <c r="B116">
-        <v>9.78727242697807</v>
+        <v>14.7516566226583</v>
       </c>
       <c r="C116">
-        <v>2.40727462237638</v>
+        <v>2.35198053450573</v>
       </c>
       <c r="D116">
-        <v>5.2125757858243</v>
+        <v>2.35671197284596</v>
       </c>
       <c r="E116">
-        <v>3.81395577180765</v>
+        <v>2.91179795760976</v>
       </c>
       <c r="F116">
-        <v>3.73142450915671</v>
+        <v>3.08133622099961</v>
       </c>
       <c r="G116">
-        <v>4.07894196425941</v>
+        <v>2.07557437853888</v>
       </c>
     </row>
     <row r="117" spans="1:7">
@@ -3071,22 +3074,22 @@
         <v>38625</v>
       </c>
       <c r="B117">
-        <v>12.2407778777725</v>
+        <v>14.7740079276007</v>
       </c>
       <c r="C117">
-        <v>2.05025803993767</v>
+        <v>2.35163418665632</v>
       </c>
       <c r="D117">
-        <v>3.84472353265561</v>
+        <v>2.35640060685144</v>
       </c>
       <c r="E117">
-        <v>3.2936581086855</v>
+        <v>2.90896542226476</v>
       </c>
       <c r="F117">
-        <v>3.71244670189317</v>
+        <v>3.0812722433388</v>
       </c>
       <c r="G117">
-        <v>3.55791580288158</v>
+        <v>2.07293113559693</v>
       </c>
     </row>
     <row r="118" spans="1:7">
@@ -3094,22 +3097,22 @@
         <v>38717</v>
       </c>
       <c r="B118">
-        <v>10.6183869640762</v>
+        <v>14.7590028669258</v>
       </c>
       <c r="C118">
-        <v>2.26712220911747</v>
+        <v>2.35818282774163</v>
       </c>
       <c r="D118">
-        <v>4.26468433837429</v>
+        <v>2.35713080730157</v>
       </c>
       <c r="E118">
-        <v>3.98158809659154</v>
+        <v>2.91269957974484</v>
       </c>
       <c r="F118">
-        <v>5.11430822847707</v>
+        <v>3.08350748651486</v>
       </c>
       <c r="G118">
-        <v>4.82193731155675</v>
+        <v>2.0680896499088</v>
       </c>
     </row>
     <row r="119" spans="1:7">
@@ -3117,22 +3120,22 @@
         <v>38807</v>
       </c>
       <c r="B119">
-        <v>12.3192076097602</v>
+        <v>14.7308825651267</v>
       </c>
       <c r="C119">
-        <v>1.99986407506721</v>
+        <v>2.35443412258722</v>
       </c>
       <c r="D119">
-        <v>5.06980195694188</v>
+        <v>2.35650559716042</v>
       </c>
       <c r="E119">
-        <v>4.05356105183295</v>
+        <v>2.90834587544859</v>
       </c>
       <c r="F119">
-        <v>3.79370429387013</v>
+        <v>3.08234163341902</v>
       </c>
       <c r="G119">
-        <v>4.52337844603932</v>
+        <v>2.07248969199938</v>
       </c>
     </row>
     <row r="120" spans="1:7">
@@ -3140,22 +3143,22 @@
         <v>38898</v>
       </c>
       <c r="B120">
-        <v>14.1065754995445</v>
+        <v>14.7565657107092</v>
       </c>
       <c r="C120">
-        <v>2.32159535137825</v>
+        <v>2.35874740342947</v>
       </c>
       <c r="D120">
-        <v>3.89515031955877</v>
+        <v>2.35846583278173</v>
       </c>
       <c r="E120">
-        <v>3.93459615700174</v>
+        <v>2.91421686109975</v>
       </c>
       <c r="F120">
-        <v>4.25252486313368</v>
+        <v>3.08478827129563</v>
       </c>
       <c r="G120">
-        <v>4.01568800231409</v>
+        <v>2.07317477077017</v>
       </c>
     </row>
     <row r="121" spans="1:7">
@@ -3163,22 +3166,22 @@
         <v>38990</v>
       </c>
       <c r="B121">
-        <v>14.6277642574987</v>
+        <v>14.7408997797024</v>
       </c>
       <c r="C121">
-        <v>2.07034940796991</v>
+        <v>2.35445679946229</v>
       </c>
       <c r="D121">
-        <v>4.62946171475853</v>
+        <v>2.35584950320915</v>
       </c>
       <c r="E121">
-        <v>4.06348802186316</v>
+        <v>2.91206316600261</v>
       </c>
       <c r="F121">
-        <v>3.74648533325757</v>
+        <v>3.08296377032271</v>
       </c>
       <c r="G121">
-        <v>4.00887134475513</v>
+        <v>2.18507576809282</v>
       </c>
     </row>
     <row r="122" spans="1:7">
@@ -3186,22 +3189,22 @@
         <v>39082</v>
       </c>
       <c r="B122">
-        <v>11.3575272095172</v>
+        <v>14.736626904497</v>
       </c>
       <c r="C122">
-        <v>2.38841004714031</v>
+        <v>2.3591401889751</v>
       </c>
       <c r="D122">
-        <v>4.06393662546109</v>
+        <v>2.35792023427886</v>
       </c>
       <c r="E122">
-        <v>4.15836920461824</v>
+        <v>2.90757638860512</v>
       </c>
       <c r="F122">
-        <v>4.41035900763511</v>
+        <v>3.08534850257241</v>
       </c>
       <c r="G122">
-        <v>4.13611195974065</v>
+        <v>2.18260421297526</v>
       </c>
     </row>
     <row r="123" spans="1:7">
@@ -3209,22 +3212,22 @@
         <v>39172</v>
       </c>
       <c r="B123">
-        <v>10.329335480536</v>
+        <v>14.7353940064192</v>
       </c>
       <c r="C123">
-        <v>2.94479093197746</v>
+        <v>2.35088886683196</v>
       </c>
       <c r="D123">
-        <v>5.86977930198434</v>
+        <v>2.3564124132556</v>
       </c>
       <c r="E123">
-        <v>4.16808543081028</v>
+        <v>2.90881332822892</v>
       </c>
       <c r="F123">
-        <v>4.1118314281286</v>
+        <v>3.08060039856709</v>
       </c>
       <c r="G123">
-        <v>3.16802427162912</v>
+        <v>2.18269384280449</v>
       </c>
     </row>
     <row r="124" spans="1:7">
@@ -3232,22 +3235,22 @@
         <v>39263</v>
       </c>
       <c r="B124">
-        <v>11.7222522422617</v>
+        <v>14.7323029862462</v>
       </c>
       <c r="C124">
-        <v>2.20550257944294</v>
+        <v>2.35358873900555</v>
       </c>
       <c r="D124">
-        <v>5.91701793145723</v>
+        <v>2.35374940399069</v>
       </c>
       <c r="E124">
-        <v>4.29403763100358</v>
+        <v>2.91234053089483</v>
       </c>
       <c r="F124">
-        <v>4.09805984068219</v>
+        <v>3.08586171483096</v>
       </c>
       <c r="G124">
-        <v>3.62325785139928</v>
+        <v>2.18319361954208</v>
       </c>
     </row>
     <row r="125" spans="1:7">
@@ -3255,22 +3258,22 @@
         <v>39355</v>
       </c>
       <c r="B125">
-        <v>12.0041349133897</v>
+        <v>13.7763544589641</v>
       </c>
       <c r="C125">
-        <v>2.28304504566336</v>
+        <v>3.52957765348839</v>
       </c>
       <c r="D125">
-        <v>5.57143860852657</v>
+        <v>2.35662260512105</v>
       </c>
       <c r="E125">
-        <v>3.72277075263055</v>
+        <v>2.57364180126509</v>
       </c>
       <c r="F125">
-        <v>3.90619117669596</v>
+        <v>3.01854723554184</v>
       </c>
       <c r="G125">
-        <v>3.91334213315094</v>
+        <v>2.11639718728952</v>
       </c>
     </row>
     <row r="126" spans="1:7">
@@ -3278,22 +3281,22 @@
         <v>39447</v>
       </c>
       <c r="B126">
-        <v>12.2240216600005</v>
+        <v>13.2089206494231</v>
       </c>
       <c r="C126">
-        <v>2.32584980309017</v>
+        <v>4.41825540754418</v>
       </c>
       <c r="D126">
-        <v>4.65869638072081</v>
+        <v>2.34615608077935</v>
       </c>
       <c r="E126">
-        <v>3.82177923296413</v>
+        <v>2.70227213293632</v>
       </c>
       <c r="F126">
-        <v>4.48443592045956</v>
+        <v>2.94076931616995</v>
       </c>
       <c r="G126">
-        <v>4.55990410518837</v>
+        <v>2.06989844015616</v>
       </c>
     </row>
     <row r="127" spans="1:7">
@@ -3301,22 +3304,22 @@
         <v>39538</v>
       </c>
       <c r="B127">
-        <v>11.3334472888218</v>
+        <v>14.8733554908907</v>
       </c>
       <c r="C127">
-        <v>2.26792233542482</v>
+        <v>6.29660139819085</v>
       </c>
       <c r="D127">
-        <v>5.48648464076359</v>
+        <v>2.35226832351462</v>
       </c>
       <c r="E127">
-        <v>3.53935087227212</v>
+        <v>2.96893034540762</v>
       </c>
       <c r="F127">
-        <v>3.89181234436383</v>
+        <v>2.88962888486002</v>
       </c>
       <c r="G127">
-        <v>4.50698707619965</v>
+        <v>2.01591805205363</v>
       </c>
     </row>
     <row r="128" spans="1:7">
@@ -3324,22 +3327,22 @@
         <v>39629</v>
       </c>
       <c r="B128">
-        <v>11.2900564329469</v>
+        <v>7.24407154782408</v>
       </c>
       <c r="C128">
-        <v>2.47631669213501</v>
+        <v>7.76668514474887</v>
       </c>
       <c r="D128">
-        <v>4.42893930331551</v>
+        <v>2.41746387455908</v>
       </c>
       <c r="E128">
-        <v>3.31117464175811</v>
+        <v>3.32046982711526</v>
       </c>
       <c r="F128">
-        <v>2.85760875014999</v>
+        <v>2.91874712252076</v>
       </c>
       <c r="G128">
-        <v>3.47080778400444</v>
+        <v>2.02133249641862</v>
       </c>
     </row>
     <row r="129" spans="1:7">
@@ -3347,22 +3350,22 @@
         <v>39721</v>
       </c>
       <c r="B129">
-        <v>12.0653539686549</v>
+        <v>6.89268062757341</v>
       </c>
       <c r="C129">
-        <v>1.91682963844789</v>
+        <v>8.96633286513119</v>
       </c>
       <c r="D129">
-        <v>5.98421324111884</v>
+        <v>2.39945713431038</v>
       </c>
       <c r="E129">
-        <v>4.84913495732669</v>
+        <v>4.17195991341733</v>
       </c>
       <c r="F129">
-        <v>4.15048804193241</v>
+        <v>3.54219573685747</v>
       </c>
       <c r="G129">
-        <v>3.8337553952258</v>
+        <v>1.95151579600104</v>
       </c>
     </row>
     <row r="130" spans="1:7">
@@ -3370,22 +3373,22 @@
         <v>39813</v>
       </c>
       <c r="B130">
-        <v>12.5319965972073</v>
+        <v>7.65310400408494</v>
       </c>
       <c r="C130">
-        <v>2.40944541978956</v>
+        <v>10.1915331302571</v>
       </c>
       <c r="D130">
-        <v>4.41662993006423</v>
+        <v>2.39783558724769</v>
       </c>
       <c r="E130">
-        <v>3.81330765899881</v>
+        <v>4.42972200939477</v>
       </c>
       <c r="F130">
-        <v>4.50697387127868</v>
+        <v>4.28841040823216</v>
       </c>
       <c r="G130">
-        <v>3.63074804508043</v>
+        <v>1.88807436257202</v>
       </c>
     </row>
     <row r="131" spans="1:7">
@@ -3393,22 +3396,22 @@
         <v>39903</v>
       </c>
       <c r="B131">
-        <v>11.4517445353526</v>
+        <v>9.16060704885234</v>
       </c>
       <c r="C131">
-        <v>2.74882377819728</v>
+        <v>6.88210653053799</v>
       </c>
       <c r="D131">
-        <v>4.9188569765167</v>
+        <v>2.38467942582057</v>
       </c>
       <c r="E131">
-        <v>4.0154736008116</v>
+        <v>3.78412278019646</v>
       </c>
       <c r="F131">
-        <v>4.21902464536363</v>
+        <v>3.32480636198042</v>
       </c>
       <c r="G131">
-        <v>3.75624656658869</v>
+        <v>1.99132936069219</v>
       </c>
     </row>
     <row r="132" spans="1:7">
@@ -3416,22 +3419,22 @@
         <v>39994</v>
       </c>
       <c r="B132">
-        <v>11.9541929646987</v>
+        <v>9.81255696490577</v>
       </c>
       <c r="C132">
-        <v>2.12905274904036</v>
+        <v>6.83628722370463</v>
       </c>
       <c r="D132">
-        <v>2.75388241779497</v>
+        <v>2.38406661819082</v>
       </c>
       <c r="E132">
-        <v>4.15687514594453</v>
+        <v>3.77483007653271</v>
       </c>
       <c r="F132">
-        <v>4.21418817360176</v>
+        <v>3.30607419797699</v>
       </c>
       <c r="G132">
-        <v>4.18107691566998</v>
+        <v>1.98353108645424</v>
       </c>
     </row>
     <row r="133" spans="1:7">
@@ -3439,22 +3442,22 @@
         <v>40086</v>
       </c>
       <c r="B133">
-        <v>11.3191739432318</v>
+        <v>6.39528028808497</v>
       </c>
       <c r="C133">
-        <v>2.72830068440271</v>
+        <v>7.02234616932953</v>
       </c>
       <c r="D133">
-        <v>5.19519791274053</v>
+        <v>2.4197786489669</v>
       </c>
       <c r="E133">
-        <v>4.00917684129727</v>
+        <v>3.63975791049447</v>
       </c>
       <c r="F133">
-        <v>4.72148953851545</v>
+        <v>3.37205281935646</v>
       </c>
       <c r="G133">
-        <v>4.11145934335373</v>
+        <v>2.02102337015311</v>
       </c>
     </row>
     <row r="134" spans="1:7">
@@ -3462,22 +3465,22 @@
         <v>40178</v>
       </c>
       <c r="B134">
-        <v>11.6234374149467</v>
+        <v>6.46681597168116</v>
       </c>
       <c r="C134">
-        <v>2.63016644415618</v>
+        <v>7.03892878782536</v>
       </c>
       <c r="D134">
-        <v>4.61342731646609</v>
+        <v>2.42284053007156</v>
       </c>
       <c r="E134">
-        <v>4.10706968958007</v>
+        <v>3.43904749929828</v>
       </c>
       <c r="F134">
-        <v>4.04315756049031</v>
+        <v>3.39304629639526</v>
       </c>
       <c r="G134">
-        <v>3.97414447935148</v>
+        <v>2.03753578250463</v>
       </c>
     </row>
     <row r="135" spans="1:7">
@@ -3485,22 +3488,22 @@
         <v>40268</v>
       </c>
       <c r="B135">
-        <v>9.43931947523402</v>
+        <v>6.58808838779368</v>
       </c>
       <c r="C135">
-        <v>2.79279167382831</v>
+        <v>7.05491337843765</v>
       </c>
       <c r="D135">
-        <v>3.7371589399399</v>
+        <v>2.42815663081737</v>
       </c>
       <c r="E135">
-        <v>3.90512315455485</v>
+        <v>3.2333386665064</v>
       </c>
       <c r="F135">
-        <v>4.37021773223612</v>
+        <v>3.42404944988035</v>
       </c>
       <c r="G135">
-        <v>3.25551631628</v>
+        <v>2.0540890746258</v>
       </c>
     </row>
     <row r="136" spans="1:7">
@@ -3508,22 +3511,22 @@
         <v>40359</v>
       </c>
       <c r="B136">
-        <v>10.4842579551711</v>
+        <v>6.50223923209407</v>
       </c>
       <c r="C136">
-        <v>2.66345506296061</v>
+        <v>7.02008737377566</v>
       </c>
       <c r="D136">
-        <v>3.87388521538458</v>
+        <v>2.4317758694532</v>
       </c>
       <c r="E136">
-        <v>3.28964251711581</v>
+        <v>3.77383962741432</v>
       </c>
       <c r="F136">
-        <v>5.40150602606423</v>
+        <v>3.39837786546103</v>
       </c>
       <c r="G136">
-        <v>3.88638693560515</v>
+        <v>2.03902636413599</v>
       </c>
     </row>
     <row r="137" spans="1:7">
@@ -3531,22 +3534,22 @@
         <v>40451</v>
       </c>
       <c r="B137">
-        <v>12.3769572780424</v>
+        <v>6.48325212456319</v>
       </c>
       <c r="C137">
-        <v>3.27356422996273</v>
+        <v>7.01218872231681</v>
       </c>
       <c r="D137">
-        <v>4.68715506133258</v>
+        <v>2.42992345053491</v>
       </c>
       <c r="E137">
-        <v>4.29252913770687</v>
+        <v>3.77329358222731</v>
       </c>
       <c r="F137">
-        <v>4.11888050282784</v>
+        <v>3.40106823776662</v>
       </c>
       <c r="G137">
-        <v>3.84899013976213</v>
+        <v>2.03814726722401</v>
       </c>
     </row>
     <row r="138" spans="1:7">
@@ -3554,22 +3557,22 @@
         <v>40543</v>
       </c>
       <c r="B138">
-        <v>11.9997710532784</v>
+        <v>6.49198001867447</v>
       </c>
       <c r="C138">
-        <v>2.84554870503415</v>
+        <v>7.02837942654263</v>
       </c>
       <c r="D138">
-        <v>4.48613707931288</v>
+        <v>2.42761241649035</v>
       </c>
       <c r="E138">
-        <v>4.63360982782511</v>
+        <v>3.77118938893192</v>
       </c>
       <c r="F138">
-        <v>4.01697013530522</v>
+        <v>3.40332921913321</v>
       </c>
       <c r="G138">
-        <v>3.736074991357</v>
+        <v>2.04118416125068</v>
       </c>
     </row>
     <row r="139" spans="1:7">
@@ -3577,22 +3580,22 @@
         <v>40633</v>
       </c>
       <c r="B139">
-        <v>14.3672803117209</v>
+        <v>6.38387200815801</v>
       </c>
       <c r="C139">
-        <v>2.86566119322598</v>
+        <v>6.97797059515085</v>
       </c>
       <c r="D139">
-        <v>5.02910419440365</v>
+        <v>2.4262205637135</v>
       </c>
       <c r="E139">
-        <v>4.48002999246862</v>
+        <v>4.6417930559092</v>
       </c>
       <c r="F139">
-        <v>3.85494149155257</v>
+        <v>3.36419754728419</v>
       </c>
       <c r="G139">
-        <v>3.34855796182267</v>
+        <v>2.02294536152682</v>
       </c>
     </row>
     <row r="140" spans="1:7">
@@ -3600,22 +3603,22 @@
         <v>40724</v>
       </c>
       <c r="B140">
-        <v>10.4052818832288</v>
+        <v>6.28312046570939</v>
       </c>
       <c r="C140">
-        <v>3.49645140400507</v>
+        <v>6.93893118936986</v>
       </c>
       <c r="D140">
-        <v>3.77960019132736</v>
+        <v>2.42122420323549</v>
       </c>
       <c r="E140">
-        <v>4.00883942035407</v>
+        <v>5.4066195737378</v>
       </c>
       <c r="F140">
-        <v>3.7634735803539</v>
+        <v>3.32686062707516</v>
       </c>
       <c r="G140">
-        <v>4.00308969976819</v>
+        <v>2.00131881017527</v>
       </c>
     </row>
     <row r="141" spans="1:7">
@@ -3623,22 +3626,22 @@
         <v>40816</v>
       </c>
       <c r="B141">
-        <v>11.7011334235016</v>
+        <v>6.48227496749567</v>
       </c>
       <c r="C141">
-        <v>3.10306909115264</v>
+        <v>7.02310560222805</v>
       </c>
       <c r="D141">
-        <v>3.99421507629492</v>
+        <v>2.43015613201928</v>
       </c>
       <c r="E141">
-        <v>4.48562285272069</v>
+        <v>3.77212654252591</v>
       </c>
       <c r="F141">
-        <v>4.51777569295699</v>
+        <v>3.40226552974352</v>
       </c>
       <c r="G141">
-        <v>3.82515230951605</v>
+        <v>2.04159117754759</v>
       </c>
     </row>
     <row r="142" spans="1:7">
@@ -3646,22 +3649,22 @@
         <v>40908</v>
       </c>
       <c r="B142">
-        <v>10.0747938844197</v>
+        <v>6.49575792860319</v>
       </c>
       <c r="C142">
-        <v>2.72620271008395</v>
+        <v>7.01487448987691</v>
       </c>
       <c r="D142">
-        <v>4.47290425994624</v>
+        <v>2.42904218017177</v>
       </c>
       <c r="E142">
-        <v>5.31024360782989</v>
+        <v>3.76861311956559</v>
       </c>
       <c r="F142">
-        <v>3.8846324060652</v>
+        <v>3.3973883329348</v>
       </c>
       <c r="G142">
-        <v>4.12165689813487</v>
+        <v>2.03931107042641</v>
       </c>
     </row>
     <row r="143" spans="1:7">
@@ -3669,22 +3672,22 @@
         <v>40999</v>
       </c>
       <c r="B143">
-        <v>10.7368328886177</v>
+        <v>6.48972434238418</v>
       </c>
       <c r="C143">
-        <v>2.94151512083769</v>
+        <v>7.01750821745167</v>
       </c>
       <c r="D143">
-        <v>5.00432991148324</v>
+        <v>2.42906776338488</v>
       </c>
       <c r="E143">
-        <v>5.18005036425344</v>
+        <v>3.77370976824559</v>
       </c>
       <c r="F143">
-        <v>3.87766076143648</v>
+        <v>3.40076824532355</v>
       </c>
       <c r="G143">
-        <v>3.96713043936254</v>
+        <v>2.04061366011677</v>
       </c>
     </row>
     <row r="144" spans="1:7">
@@ -3692,22 +3695,22 @@
         <v>41090</v>
       </c>
       <c r="B144">
-        <v>10.6167509905429</v>
+        <v>6.49184380489855</v>
       </c>
       <c r="C144">
-        <v>3.00156329838146</v>
+        <v>7.02461388147967</v>
       </c>
       <c r="D144">
-        <v>4.21160665946093</v>
+        <v>2.4260487042651</v>
       </c>
       <c r="E144">
-        <v>5.261734945845</v>
+        <v>3.77120878840974</v>
       </c>
       <c r="F144">
-        <v>3.8286117327925</v>
+        <v>3.39375555309664</v>
       </c>
       <c r="G144">
-        <v>4.02319759681293</v>
+        <v>2.04069953047182</v>
       </c>
     </row>
     <row r="145" spans="1:7">
@@ -3715,22 +3718,22 @@
         <v>41182</v>
       </c>
       <c r="B145">
-        <v>7.24929566998032</v>
+        <v>6.48382236121709</v>
       </c>
       <c r="C145">
-        <v>3.12123953004945</v>
+        <v>7.0223996522278</v>
       </c>
       <c r="D145">
-        <v>5.34062386990475</v>
+        <v>2.43235346544811</v>
       </c>
       <c r="E145">
-        <v>5.10549220717173</v>
+        <v>3.77690402954623</v>
       </c>
       <c r="F145">
-        <v>3.49971507269597</v>
+        <v>3.40032432331636</v>
       </c>
       <c r="G145">
-        <v>2.87486818124099</v>
+        <v>2.03822878485837</v>
       </c>
     </row>
     <row r="146" spans="1:7">
@@ -3738,22 +3741,22 @@
         <v>41274</v>
       </c>
       <c r="B146">
-        <v>10.4304722696555</v>
+        <v>6.48734519159376</v>
       </c>
       <c r="C146">
-        <v>3.04485506239606</v>
+        <v>7.03283600996518</v>
       </c>
       <c r="D146">
-        <v>4.61619180080971</v>
+        <v>2.43147995172091</v>
       </c>
       <c r="E146">
-        <v>5.13065290063415</v>
+        <v>3.77065797578776</v>
       </c>
       <c r="F146">
-        <v>3.51676539713174</v>
+        <v>3.39704690586281</v>
       </c>
       <c r="G146">
-        <v>2.94623516008627</v>
+        <v>2.03887534920959</v>
       </c>
     </row>
     <row r="147" spans="1:7">
@@ -3761,22 +3764,22 @@
         <v>41364</v>
       </c>
       <c r="B147">
-        <v>10.6657335112241</v>
+        <v>6.48342474544008</v>
       </c>
       <c r="C147">
-        <v>3.54589977313757</v>
+        <v>7.01956725430477</v>
       </c>
       <c r="D147">
-        <v>3.40536909463198</v>
+        <v>2.43165398735347</v>
       </c>
       <c r="E147">
-        <v>5.37653888063088</v>
+        <v>3.77620921622756</v>
       </c>
       <c r="F147">
-        <v>3.95769638457483</v>
+        <v>3.40236840094418</v>
       </c>
       <c r="G147">
-        <v>3.57257433992796</v>
+        <v>2.0416509372422</v>
       </c>
     </row>
     <row r="148" spans="1:7">
@@ -3784,22 +3787,22 @@
         <v>41455</v>
       </c>
       <c r="B148">
-        <v>10.6516997078114</v>
+        <v>6.49070531988801</v>
       </c>
       <c r="C148">
-        <v>4.19504830605255</v>
+        <v>7.02267508487144</v>
       </c>
       <c r="D148">
-        <v>4.46112010136758</v>
+        <v>2.43018692109883</v>
       </c>
       <c r="E148">
-        <v>4.44233426991344</v>
+        <v>3.77637482429885</v>
       </c>
       <c r="F148">
-        <v>3.69668526211821</v>
+        <v>3.40155336947342</v>
       </c>
       <c r="G148">
-        <v>3.88858589290992</v>
+        <v>2.04254329335243</v>
       </c>
     </row>
     <row r="149" spans="1:7">
@@ -3807,22 +3810,22 @@
         <v>41547</v>
       </c>
       <c r="B149">
-        <v>11.8423866038517</v>
+        <v>6.48638322038575</v>
       </c>
       <c r="C149">
-        <v>3.7786956513475</v>
+        <v>7.01796322713568</v>
       </c>
       <c r="D149">
-        <v>5.62771244692227</v>
+        <v>2.42704325669527</v>
       </c>
       <c r="E149">
-        <v>4.81114768136143</v>
+        <v>3.77254396190994</v>
       </c>
       <c r="F149">
-        <v>3.4678712526247</v>
+        <v>3.40135987672593</v>
       </c>
       <c r="G149">
-        <v>2.94827919773521</v>
+        <v>2.04079663216687</v>
       </c>
     </row>
     <row r="150" spans="1:7">
@@ -3830,22 +3833,22 @@
         <v>41639</v>
       </c>
       <c r="B150">
-        <v>12.1336308030493</v>
+        <v>6.49181994698559</v>
       </c>
       <c r="C150">
-        <v>4.84008733465031</v>
+        <v>7.02653741415233</v>
       </c>
       <c r="D150">
-        <v>5.37687194127977</v>
+        <v>2.42967352770797</v>
       </c>
       <c r="E150">
-        <v>4.73413473055134</v>
+        <v>3.76725877325489</v>
       </c>
       <c r="F150">
-        <v>3.49636103284245</v>
+        <v>3.39378301831919</v>
       </c>
       <c r="G150">
-        <v>3.3551699508253</v>
+        <v>2.03831580936796</v>
       </c>
     </row>
     <row r="151" spans="1:7">
@@ -3853,22 +3856,22 @@
         <v>41729</v>
       </c>
       <c r="B151">
-        <v>9.53606306639393</v>
+        <v>6.48964407632198</v>
       </c>
       <c r="C151">
-        <v>3.76388856320154</v>
+        <v>7.02197077592505</v>
       </c>
       <c r="D151">
-        <v>3.17277833922509</v>
+        <v>2.43060292138842</v>
       </c>
       <c r="E151">
-        <v>4.26819880333316</v>
+        <v>3.77062046702332</v>
       </c>
       <c r="F151">
-        <v>3.1726904172947</v>
+        <v>3.39705970053854</v>
       </c>
       <c r="G151">
-        <v>4.23611314186277</v>
+        <v>2.04342506607787</v>
       </c>
     </row>
     <row r="152" spans="1:7">
@@ -3876,22 +3879,22 @@
         <v>41820</v>
       </c>
       <c r="B152">
-        <v>11.1450336290659</v>
+        <v>6.48423540206795</v>
       </c>
       <c r="C152">
-        <v>4.58961072093835</v>
+        <v>7.0218178392485</v>
       </c>
       <c r="D152">
-        <v>4.68383003122085</v>
+        <v>2.42992413010371</v>
       </c>
       <c r="E152">
-        <v>4.44365485494821</v>
+        <v>3.77148286667637</v>
       </c>
       <c r="F152">
-        <v>3.34939985852716</v>
+        <v>3.39704781235491</v>
       </c>
       <c r="G152">
-        <v>3.57010782716406</v>
+        <v>2.03844672896519</v>
       </c>
     </row>
     <row r="153" spans="1:7">
@@ -3899,22 +3902,22 @@
         <v>41912</v>
       </c>
       <c r="B153">
-        <v>12.2782821812713</v>
+        <v>6.48648183326006</v>
       </c>
       <c r="C153">
-        <v>3.35800758776491</v>
+        <v>7.02339379910271</v>
       </c>
       <c r="D153">
-        <v>5.37587926255418</v>
+        <v>2.42798987413013</v>
       </c>
       <c r="E153">
-        <v>6.21710038130519</v>
+        <v>3.76908281898501</v>
       </c>
       <c r="F153">
-        <v>4.2669409655492</v>
+        <v>3.39869623817611</v>
       </c>
       <c r="G153">
-        <v>2.94728574703815</v>
+        <v>2.04079301636451</v>
       </c>
     </row>
     <row r="154" spans="1:7">
@@ -3922,22 +3925,22 @@
         <v>42004</v>
       </c>
       <c r="B154">
-        <v>9.72489321580399</v>
+        <v>6.49262493500085</v>
       </c>
       <c r="C154">
-        <v>4.07507052784755</v>
+        <v>7.02207840656475</v>
       </c>
       <c r="D154">
-        <v>4.26889431325478</v>
+        <v>2.42907789983987</v>
       </c>
       <c r="E154">
-        <v>5.95403824379958</v>
+        <v>3.77684859057105</v>
       </c>
       <c r="F154">
-        <v>3.6466002983841</v>
+        <v>3.39699596320814</v>
       </c>
       <c r="G154">
-        <v>3.35018562879391</v>
+        <v>2.04122968227399</v>
       </c>
     </row>
     <row r="155" spans="1:7">
@@ -3945,22 +3948,22 @@
         <v>42094</v>
       </c>
       <c r="B155">
-        <v>12.4125788076886</v>
+        <v>6.48464977226198</v>
       </c>
       <c r="C155">
-        <v>2.94828864103295</v>
+        <v>7.01754379956616</v>
       </c>
       <c r="D155">
-        <v>3.68537930974593</v>
+        <v>2.43085895984632</v>
       </c>
       <c r="E155">
-        <v>4.23769056997784</v>
+        <v>3.77260938885586</v>
       </c>
       <c r="F155">
-        <v>4.26280317679003</v>
+        <v>3.3980562773747</v>
       </c>
       <c r="G155">
-        <v>3.18029519458436</v>
+        <v>2.04019421288782</v>
       </c>
     </row>
     <row r="156" spans="1:7">
@@ -3968,22 +3971,22 @@
         <v>42185</v>
       </c>
       <c r="B156">
-        <v>5.4046228865403</v>
+        <v>6.31322256791835</v>
       </c>
       <c r="C156">
-        <v>2.02830205527396</v>
+        <v>6.95595931870526</v>
       </c>
       <c r="D156">
-        <v>3.29984412221926</v>
+        <v>2.42242438650855</v>
       </c>
       <c r="E156">
-        <v>5.45875688170999</v>
+        <v>3.7287661326981</v>
       </c>
       <c r="F156">
-        <v>4.39389827519885</v>
+        <v>3.96027959185417</v>
       </c>
       <c r="G156">
-        <v>4.30588530898568</v>
+        <v>2.01941717881105</v>
       </c>
     </row>
     <row r="157" spans="1:7">
@@ -3991,22 +3994,22 @@
         <v>42277</v>
       </c>
       <c r="B157">
-        <v>10.4721601163809</v>
+        <v>6.31753074027358</v>
       </c>
       <c r="C157">
-        <v>3.05630365795046</v>
+        <v>6.95420142854867</v>
       </c>
       <c r="D157">
-        <v>4.86532849681628</v>
+        <v>2.42960588004845</v>
       </c>
       <c r="E157">
-        <v>5.33493305315311</v>
+        <v>3.72955922277593</v>
       </c>
       <c r="F157">
-        <v>3.92904660158065</v>
+        <v>3.96348369468333</v>
       </c>
       <c r="G157">
-        <v>3.45441722087242</v>
+        <v>2.01594797773788</v>
       </c>
     </row>
   </sheetData>

</xml_diff>